<commit_message>
Modify maximum stock number
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C5A6F1-2976-4A46-9912-BEF7980D241E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DA01E5-C312-47D5-B33E-B51291D251F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3200,7 +3200,7 @@
   <dimension ref="A2:BD259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3375,7 +3375,7 @@
         <v>104</v>
       </c>
       <c r="E7" s="32">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F7" t="s">
         <v>97</v>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="32">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>97</v>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="32">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>97</v>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="32">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F16" s="27" t="s">
         <v>97</v>
@@ -4263,112 +4263,112 @@
         <v>145</v>
       </c>
       <c r="H16" s="36">
-        <f>H29*1.12</f>
-        <v>24.245760000000004</v>
+        <f>H29*1.15</f>
+        <v>24.895200000000003</v>
       </c>
       <c r="I16" s="36">
-        <f t="shared" ref="I16:AH16" si="6">I29*1.12</f>
-        <v>0.43680000000000008</v>
+        <f t="shared" ref="I16:AH16" si="6">I29*1.15</f>
+        <v>0.44849999999999995</v>
       </c>
       <c r="J16" s="36">
         <f t="shared" si="6"/>
-        <v>4.3489600000000008</v>
+        <v>4.4654499999999997</v>
       </c>
       <c r="K16" s="36">
         <f t="shared" si="6"/>
-        <v>1.2454400000000003</v>
+        <v>1.2787999999999999</v>
       </c>
       <c r="L16" s="36">
         <f t="shared" si="6"/>
-        <v>0.79856000000000005</v>
+        <v>0.81994999999999985</v>
       </c>
       <c r="M16" s="36">
         <f t="shared" si="6"/>
-        <v>0.50960000000000005</v>
+        <v>0.52324999999999999</v>
       </c>
       <c r="N16" s="36">
         <f t="shared" si="6"/>
-        <v>0.30912000000000006</v>
+        <v>0.31740000000000002</v>
       </c>
       <c r="O16" s="36">
         <f t="shared" si="6"/>
-        <v>0.6910400000000001</v>
+        <v>0.7095499999999999</v>
       </c>
       <c r="P16" s="36">
         <f t="shared" si="6"/>
-        <v>1.5948800000000001</v>
+        <v>1.6375999999999997</v>
       </c>
       <c r="Q16" s="36">
         <f t="shared" si="6"/>
-        <v>0.36176000000000003</v>
+        <v>0.37145</v>
       </c>
       <c r="R16" s="36">
         <f t="shared" si="6"/>
-        <v>0.35392000000000001</v>
+        <v>0.3634</v>
       </c>
       <c r="S16" s="36">
         <f t="shared" si="6"/>
-        <v>1.5568</v>
+        <v>1.5984999999999998</v>
       </c>
       <c r="T16" s="36">
         <f t="shared" si="6"/>
-        <v>0.44352000000000008</v>
+        <v>0.45539999999999997</v>
       </c>
       <c r="U16" s="36">
         <f t="shared" si="6"/>
-        <v>0.44464000000000009</v>
+        <v>0.45655000000000001</v>
       </c>
       <c r="V16" s="36">
         <f t="shared" si="6"/>
-        <v>2.86496</v>
+        <v>2.9416999999999995</v>
       </c>
       <c r="W16" s="36">
         <f t="shared" si="6"/>
-        <v>0.5779200000000001</v>
+        <v>0.59339999999999993</v>
       </c>
       <c r="X16" s="36">
         <f t="shared" si="6"/>
-        <v>1.05392</v>
+        <v>1.0821499999999999</v>
       </c>
       <c r="Y16" s="36">
         <f t="shared" si="6"/>
-        <v>1.1760000000000002</v>
+        <v>1.2075</v>
       </c>
       <c r="Z16" s="36">
         <f t="shared" si="6"/>
-        <v>0.40096000000000004</v>
+        <v>0.41169999999999995</v>
       </c>
       <c r="AA16" s="36">
         <f t="shared" si="6"/>
-        <v>1.1491200000000001</v>
+        <v>1.1798999999999999</v>
       </c>
       <c r="AB16" s="36">
         <f t="shared" si="6"/>
-        <v>0.15120000000000003</v>
+        <v>0.15525</v>
       </c>
       <c r="AC16" s="36">
         <f t="shared" si="6"/>
-        <v>0.63839999999999997</v>
+        <v>0.65549999999999986</v>
       </c>
       <c r="AD16" s="36">
         <f t="shared" si="6"/>
-        <v>0.36512000000000006</v>
+        <v>0.37490000000000001</v>
       </c>
       <c r="AE16" s="36">
         <f t="shared" si="6"/>
-        <v>0.25984000000000002</v>
+        <v>0.26679999999999998</v>
       </c>
       <c r="AF16" s="36">
         <f t="shared" si="6"/>
-        <v>0.54656000000000005</v>
+        <v>0.56119999999999992</v>
       </c>
       <c r="AG16" s="36">
         <f t="shared" si="6"/>
-        <v>0.80640000000000001</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="AH16" s="36">
         <f t="shared" si="6"/>
-        <v>1.1603200000000002</v>
+        <v>1.1914</v>
       </c>
       <c r="AI16" s="19">
         <v>0</v>
@@ -4389,111 +4389,111 @@
       <c r="G17" s="34"/>
       <c r="H17" s="26">
         <f>H16*2.4</f>
-        <v>58.189824000000009</v>
+        <v>59.748480000000001</v>
       </c>
       <c r="I17" s="26">
         <f t="shared" ref="I17:AH17" si="7">I16*2.4</f>
-        <v>1.0483200000000001</v>
+        <v>1.0763999999999998</v>
       </c>
       <c r="J17" s="26">
         <f t="shared" si="7"/>
-        <v>10.437504000000002</v>
+        <v>10.717079999999999</v>
       </c>
       <c r="K17" s="26">
         <f t="shared" si="7"/>
-        <v>2.9890560000000006</v>
+        <v>3.0691199999999998</v>
       </c>
       <c r="L17" s="26">
         <f t="shared" si="7"/>
-        <v>1.916544</v>
+        <v>1.9678799999999996</v>
       </c>
       <c r="M17" s="26">
         <f t="shared" si="7"/>
-        <v>1.2230400000000001</v>
+        <v>1.2558</v>
       </c>
       <c r="N17" s="26">
         <f t="shared" si="7"/>
-        <v>0.7418880000000001</v>
+        <v>0.76175999999999999</v>
       </c>
       <c r="O17" s="26">
         <f t="shared" si="7"/>
-        <v>1.6584960000000002</v>
+        <v>1.7029199999999998</v>
       </c>
       <c r="P17" s="26">
         <f t="shared" si="7"/>
-        <v>3.827712</v>
+        <v>3.9302399999999991</v>
       </c>
       <c r="Q17" s="26">
         <f t="shared" si="7"/>
-        <v>0.868224</v>
+        <v>0.89147999999999994</v>
       </c>
       <c r="R17" s="26">
         <f t="shared" si="7"/>
-        <v>0.84940800000000005</v>
+        <v>0.87215999999999994</v>
       </c>
       <c r="S17" s="26">
         <f t="shared" si="7"/>
-        <v>3.7363199999999996</v>
+        <v>3.8363999999999994</v>
       </c>
       <c r="T17" s="26">
         <f t="shared" si="7"/>
-        <v>1.0644480000000001</v>
+        <v>1.0929599999999999</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="7"/>
-        <v>1.0671360000000001</v>
+        <v>1.09572</v>
       </c>
       <c r="V17" s="26">
         <f t="shared" si="7"/>
-        <v>6.8759039999999993</v>
+        <v>7.0600799999999984</v>
       </c>
       <c r="W17" s="26">
         <f t="shared" si="7"/>
-        <v>1.3870080000000002</v>
+        <v>1.4241599999999999</v>
       </c>
       <c r="X17" s="26">
         <f t="shared" si="7"/>
-        <v>2.5294079999999997</v>
+        <v>2.5971599999999997</v>
       </c>
       <c r="Y17" s="26">
         <f t="shared" si="7"/>
-        <v>2.8224000000000005</v>
+        <v>2.8980000000000001</v>
       </c>
       <c r="Z17" s="26">
         <f t="shared" si="7"/>
-        <v>0.96230400000000005</v>
+        <v>0.98807999999999985</v>
       </c>
       <c r="AA17" s="26">
         <f t="shared" si="7"/>
-        <v>2.7578880000000003</v>
+        <v>2.8317599999999996</v>
       </c>
       <c r="AB17" s="26">
         <f t="shared" si="7"/>
-        <v>0.36288000000000004</v>
+        <v>0.37259999999999999</v>
       </c>
       <c r="AC17" s="26">
         <f t="shared" si="7"/>
-        <v>1.53216</v>
+        <v>1.5731999999999997</v>
       </c>
       <c r="AD17" s="26">
         <f t="shared" si="7"/>
-        <v>0.87628800000000007</v>
+        <v>0.89976</v>
       </c>
       <c r="AE17" s="26">
         <f t="shared" si="7"/>
-        <v>0.62361600000000006</v>
+        <v>0.64031999999999989</v>
       </c>
       <c r="AF17" s="26">
         <f t="shared" si="7"/>
-        <v>1.311744</v>
+        <v>1.3468799999999999</v>
       </c>
       <c r="AG17" s="26">
         <f t="shared" si="7"/>
-        <v>1.93536</v>
+        <v>1.9871999999999999</v>
       </c>
       <c r="AH17" s="26">
         <f t="shared" si="7"/>
-        <v>2.7847680000000006</v>
+        <v>2.8593600000000001</v>
       </c>
       <c r="AI17" s="19">
         <v>0</v>

</xml_diff>

<commit_message>
Modify maximum stock number for HGT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CAC0B1-753D-4FBC-ACE7-5DBC3D5AE721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6F22D7-2FBE-470C-84D2-E2A832D704A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3202,8 +3202,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="Q13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:AH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5986,112 +5986,112 @@
       </c>
       <c r="G30" s="32"/>
       <c r="H30" s="34">
-        <f>H29*1.2</f>
-        <v>28.575360000000007</v>
+        <f>H29*1.3</f>
+        <v>30.956640000000011</v>
       </c>
       <c r="I30" s="34">
-        <f t="shared" ref="I30:AH30" si="17">I29*1.2</f>
-        <v>0.51480000000000004</v>
+        <f t="shared" ref="I30:AH30" si="17">I29*1.3</f>
+        <v>0.55770000000000008</v>
       </c>
       <c r="J30" s="34">
         <f t="shared" si="17"/>
-        <v>5.1255600000000001</v>
+        <v>5.5526900000000001</v>
       </c>
       <c r="K30" s="34">
         <f t="shared" si="17"/>
-        <v>1.4678400000000003</v>
+        <v>1.5901600000000005</v>
       </c>
       <c r="L30" s="34">
         <f t="shared" si="17"/>
-        <v>0.94116</v>
+        <v>1.01959</v>
       </c>
       <c r="M30" s="34">
         <f t="shared" si="17"/>
-        <v>0.60060000000000002</v>
+        <v>0.65065000000000006</v>
       </c>
       <c r="N30" s="34">
         <f t="shared" si="17"/>
-        <v>0.36432000000000003</v>
+        <v>0.39468000000000009</v>
       </c>
       <c r="O30" s="34">
         <f t="shared" si="17"/>
-        <v>0.81444000000000005</v>
+        <v>0.88231000000000015</v>
       </c>
       <c r="P30" s="34">
         <f t="shared" si="17"/>
-        <v>1.87968</v>
+        <v>2.0363199999999999</v>
       </c>
       <c r="Q30" s="34">
         <f t="shared" si="17"/>
-        <v>0.42636000000000007</v>
+        <v>0.46189000000000008</v>
       </c>
       <c r="R30" s="34">
         <f t="shared" si="17"/>
-        <v>0.41711999999999999</v>
+        <v>0.45188000000000006</v>
       </c>
       <c r="S30" s="34">
         <f t="shared" si="17"/>
-        <v>1.8347999999999998</v>
+        <v>1.9877</v>
       </c>
       <c r="T30" s="34">
         <f t="shared" si="17"/>
-        <v>0.52272000000000007</v>
+        <v>0.56628000000000012</v>
       </c>
       <c r="U30" s="34">
         <f t="shared" si="17"/>
-        <v>0.52404000000000006</v>
+        <v>0.56771000000000005</v>
       </c>
       <c r="V30" s="34">
         <f t="shared" si="17"/>
-        <v>3.37656</v>
+        <v>3.6579400000000004</v>
       </c>
       <c r="W30" s="34">
         <f t="shared" si="17"/>
-        <v>0.68112000000000006</v>
+        <v>0.7378800000000002</v>
       </c>
       <c r="X30" s="34">
         <f t="shared" si="17"/>
-        <v>1.2421200000000001</v>
+        <v>1.3456300000000003</v>
       </c>
       <c r="Y30" s="34">
         <f t="shared" si="17"/>
-        <v>1.3860000000000003</v>
+        <v>1.5015000000000003</v>
       </c>
       <c r="Z30" s="34">
         <f t="shared" si="17"/>
-        <v>0.47256000000000004</v>
+        <v>0.51194000000000006</v>
       </c>
       <c r="AA30" s="34">
         <f t="shared" si="17"/>
-        <v>1.35432</v>
+        <v>1.4671800000000002</v>
       </c>
       <c r="AB30" s="34">
         <f t="shared" si="17"/>
-        <v>0.17820000000000003</v>
+        <v>0.19305000000000003</v>
       </c>
       <c r="AC30" s="34">
         <f t="shared" si="17"/>
-        <v>0.75239999999999996</v>
+        <v>0.81510000000000005</v>
       </c>
       <c r="AD30" s="34">
         <f t="shared" si="17"/>
-        <v>0.43032000000000004</v>
+        <v>0.46618000000000004</v>
       </c>
       <c r="AE30" s="34">
         <f t="shared" si="17"/>
-        <v>0.30624000000000001</v>
+        <v>0.33176000000000005</v>
       </c>
       <c r="AF30" s="34">
         <f t="shared" si="17"/>
-        <v>0.64416000000000007</v>
+        <v>0.69784000000000013</v>
       </c>
       <c r="AG30" s="34">
         <f t="shared" si="17"/>
-        <v>0.95040000000000002</v>
+        <v>1.0296000000000001</v>
       </c>
       <c r="AH30" s="34">
         <f t="shared" si="17"/>
-        <v>1.3675200000000001</v>
+        <v>1.4814800000000004</v>
       </c>
       <c r="AI30" s="32"/>
     </row>
@@ -6105,112 +6105,112 @@
       </c>
       <c r="G31" s="32"/>
       <c r="H31" s="34">
-        <f>H30*1.8</f>
-        <v>51.435648000000015</v>
+        <f>H30*1.9</f>
+        <v>58.817616000000015</v>
       </c>
       <c r="I31" s="34">
-        <f t="shared" ref="I31:AH31" si="18">I30*1.8</f>
-        <v>0.92664000000000013</v>
+        <f t="shared" ref="I31:AH31" si="18">I30*1.9</f>
+        <v>1.0596300000000001</v>
       </c>
       <c r="J31" s="34">
         <f t="shared" si="18"/>
-        <v>9.2260080000000002</v>
+        <v>10.550110999999999</v>
       </c>
       <c r="K31" s="34">
         <f t="shared" si="18"/>
-        <v>2.6421120000000005</v>
+        <v>3.0213040000000007</v>
       </c>
       <c r="L31" s="34">
         <f t="shared" si="18"/>
-        <v>1.694088</v>
+        <v>1.9372209999999999</v>
       </c>
       <c r="M31" s="34">
         <f t="shared" si="18"/>
-        <v>1.08108</v>
+        <v>1.236235</v>
       </c>
       <c r="N31" s="34">
         <f t="shared" si="18"/>
-        <v>0.65577600000000003</v>
+        <v>0.74989200000000011</v>
       </c>
       <c r="O31" s="34">
         <f t="shared" si="18"/>
-        <v>1.4659920000000002</v>
+        <v>1.6763890000000001</v>
       </c>
       <c r="P31" s="34">
         <f t="shared" si="18"/>
-        <v>3.3834240000000002</v>
+        <v>3.8690079999999996</v>
       </c>
       <c r="Q31" s="34">
         <f t="shared" si="18"/>
-        <v>0.76744800000000013</v>
+        <v>0.87759100000000012</v>
       </c>
       <c r="R31" s="34">
         <f t="shared" si="18"/>
-        <v>0.75081600000000004</v>
+        <v>0.85857200000000011</v>
       </c>
       <c r="S31" s="34">
         <f t="shared" si="18"/>
-        <v>3.3026399999999998</v>
+        <v>3.7766299999999999</v>
       </c>
       <c r="T31" s="34">
         <f t="shared" si="18"/>
-        <v>0.94089600000000018</v>
+        <v>1.0759320000000001</v>
       </c>
       <c r="U31" s="34">
         <f t="shared" si="18"/>
-        <v>0.94327200000000011</v>
+        <v>1.078649</v>
       </c>
       <c r="V31" s="34">
         <f t="shared" si="18"/>
-        <v>6.0778080000000001</v>
+        <v>6.9500860000000007</v>
       </c>
       <c r="W31" s="34">
         <f t="shared" si="18"/>
-        <v>1.2260160000000002</v>
+        <v>1.4019720000000002</v>
       </c>
       <c r="X31" s="34">
         <f t="shared" si="18"/>
-        <v>2.2358160000000002</v>
+        <v>2.5566970000000007</v>
       </c>
       <c r="Y31" s="34">
         <f t="shared" si="18"/>
-        <v>2.4948000000000006</v>
+        <v>2.8528500000000006</v>
       </c>
       <c r="Z31" s="34">
         <f t="shared" si="18"/>
-        <v>0.85060800000000003</v>
+        <v>0.97268600000000005</v>
       </c>
       <c r="AA31" s="34">
         <f t="shared" si="18"/>
-        <v>2.4377759999999999</v>
+        <v>2.787642</v>
       </c>
       <c r="AB31" s="34">
         <f t="shared" si="18"/>
-        <v>0.32076000000000005</v>
+        <v>0.36679500000000004</v>
       </c>
       <c r="AC31" s="34">
         <f t="shared" si="18"/>
-        <v>1.35432</v>
+        <v>1.5486900000000001</v>
       </c>
       <c r="AD31" s="34">
         <f t="shared" si="18"/>
-        <v>0.77457600000000004</v>
+        <v>0.88574200000000003</v>
       </c>
       <c r="AE31" s="34">
         <f t="shared" si="18"/>
-        <v>0.55123200000000006</v>
+        <v>0.63034400000000013</v>
       </c>
       <c r="AF31" s="34">
         <f t="shared" si="18"/>
-        <v>1.1594880000000001</v>
+        <v>1.3258960000000002</v>
       </c>
       <c r="AG31" s="34">
         <f t="shared" si="18"/>
-        <v>1.71072</v>
+        <v>1.95624</v>
       </c>
       <c r="AH31" s="34">
         <f t="shared" si="18"/>
-        <v>2.4615360000000002</v>
+        <v>2.8148120000000008</v>
       </c>
       <c r="AI31" s="32"/>
     </row>

</xml_diff>

<commit_message>
Modify Max stock for MGT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6F22D7-2FBE-470C-84D2-E2A832D704A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A010B85-ABAB-4381-826E-CDF63637366F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3202,8 +3202,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:AH31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5193,112 +5193,112 @@
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="34">
-        <f>H22*1.25</f>
-        <v>14.483437500000001</v>
+        <f>H22*1.3</f>
+        <v>15.062775</v>
       </c>
       <c r="I23" s="34">
-        <f t="shared" ref="I23:AH23" si="12">I22*1.25</f>
-        <v>0.19293749999999998</v>
+        <f t="shared" ref="I23:AH23" si="12">I22*1.3</f>
+        <v>0.200655</v>
       </c>
       <c r="J23" s="34">
         <f t="shared" si="12"/>
-        <v>3.8928750000000005</v>
+        <v>4.0485900000000008</v>
       </c>
       <c r="K23" s="34">
         <f t="shared" si="12"/>
-        <v>0.72581250000000019</v>
+        <v>0.75484500000000021</v>
       </c>
       <c r="L23" s="34">
         <f t="shared" si="12"/>
-        <v>0.32681250000000001</v>
+        <v>0.33988500000000005</v>
       </c>
       <c r="M23" s="34">
         <f t="shared" si="12"/>
-        <v>0.28481250000000002</v>
+        <v>0.296205</v>
       </c>
       <c r="N23" s="34">
         <f t="shared" si="12"/>
-        <v>0.17587500000000003</v>
+        <v>0.18291000000000004</v>
       </c>
       <c r="O23" s="34">
         <f t="shared" si="12"/>
-        <v>0.48825000000000002</v>
+        <v>0.50778000000000001</v>
       </c>
       <c r="P23" s="34">
         <f t="shared" si="12"/>
-        <v>0.62868750000000007</v>
+        <v>0.65383500000000006</v>
       </c>
       <c r="Q23" s="34">
         <f t="shared" si="12"/>
-        <v>0.21787500000000001</v>
+        <v>0.22659000000000001</v>
       </c>
       <c r="R23" s="34">
         <f t="shared" si="12"/>
-        <v>0.25987500000000002</v>
+        <v>0.27027000000000007</v>
       </c>
       <c r="S23" s="34">
         <f t="shared" si="12"/>
-        <v>0.51056250000000003</v>
+        <v>0.53098500000000004</v>
       </c>
       <c r="T23" s="34">
         <f t="shared" si="12"/>
-        <v>0.27168749999999997</v>
+        <v>0.282555</v>
       </c>
       <c r="U23" s="34">
         <f t="shared" si="12"/>
-        <v>0.28875000000000001</v>
+        <v>0.30030000000000001</v>
       </c>
       <c r="V23" s="34">
         <f t="shared" si="12"/>
-        <v>1.5316875000000003</v>
+        <v>1.5929550000000003</v>
       </c>
       <c r="W23" s="34">
         <f t="shared" si="12"/>
-        <v>0.34387500000000004</v>
+        <v>0.35763</v>
       </c>
       <c r="X23" s="34">
         <f t="shared" si="12"/>
-        <v>0.91874999999999996</v>
+        <v>0.95550000000000002</v>
       </c>
       <c r="Y23" s="34">
         <f t="shared" si="12"/>
-        <v>0.53681250000000003</v>
+        <v>0.55828500000000003</v>
       </c>
       <c r="Z23" s="34">
         <f t="shared" si="12"/>
-        <v>0.27168749999999997</v>
+        <v>0.282555</v>
       </c>
       <c r="AA23" s="34">
         <f t="shared" si="12"/>
-        <v>0.71793750000000001</v>
+        <v>0.74665500000000007</v>
       </c>
       <c r="AB23" s="34">
         <f t="shared" si="12"/>
-        <v>9.7125000000000003E-2</v>
+        <v>0.10101000000000002</v>
       </c>
       <c r="AC23" s="34">
         <f t="shared" si="12"/>
-        <v>0.34256249999999999</v>
+        <v>0.35626500000000005</v>
       </c>
       <c r="AD23" s="34">
         <f t="shared" si="12"/>
-        <v>0.19425000000000001</v>
+        <v>0.20202000000000003</v>
       </c>
       <c r="AE23" s="34">
         <f t="shared" si="12"/>
-        <v>0.26906249999999998</v>
+        <v>0.27982499999999999</v>
       </c>
       <c r="AF23" s="34">
         <f t="shared" si="12"/>
-        <v>0.24150000000000002</v>
+        <v>0.25116000000000005</v>
       </c>
       <c r="AG23" s="34">
         <f t="shared" si="12"/>
-        <v>0.41737500000000005</v>
+        <v>0.43407000000000007</v>
       </c>
       <c r="AH23" s="34">
         <f t="shared" si="12"/>
-        <v>0.33600000000000008</v>
+        <v>0.34944000000000008</v>
       </c>
       <c r="AI23" s="32"/>
     </row>
@@ -5312,112 +5312,112 @@
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="34">
-        <f>H23*1.8</f>
-        <v>26.070187500000003</v>
+        <f>H23*2.3</f>
+        <v>34.644382499999999</v>
       </c>
       <c r="I24" s="34">
-        <f t="shared" ref="I24:AH24" si="13">I23*1.8</f>
-        <v>0.34728749999999997</v>
+        <f t="shared" ref="I24:AH24" si="13">I23*2.3</f>
+        <v>0.46150649999999999</v>
       </c>
       <c r="J24" s="34">
         <f t="shared" si="13"/>
-        <v>7.007175000000001</v>
+        <v>9.3117570000000018</v>
       </c>
       <c r="K24" s="34">
         <f t="shared" si="13"/>
-        <v>1.3064625000000003</v>
+        <v>1.7361435000000003</v>
       </c>
       <c r="L24" s="34">
         <f t="shared" si="13"/>
-        <v>0.58826250000000002</v>
+        <v>0.78173550000000003</v>
       </c>
       <c r="M24" s="34">
         <f t="shared" si="13"/>
-        <v>0.51266250000000002</v>
+        <v>0.68127149999999992</v>
       </c>
       <c r="N24" s="34">
         <f t="shared" si="13"/>
-        <v>0.31657500000000005</v>
+        <v>0.42069300000000009</v>
       </c>
       <c r="O24" s="34">
         <f t="shared" si="13"/>
-        <v>0.87885000000000002</v>
+        <v>1.167894</v>
       </c>
       <c r="P24" s="34">
         <f t="shared" si="13"/>
-        <v>1.1316375000000001</v>
+        <v>1.5038205</v>
       </c>
       <c r="Q24" s="34">
         <f t="shared" si="13"/>
-        <v>0.39217500000000005</v>
+        <v>0.52115699999999998</v>
       </c>
       <c r="R24" s="34">
         <f t="shared" si="13"/>
-        <v>0.46777500000000005</v>
+        <v>0.62162100000000009</v>
       </c>
       <c r="S24" s="34">
         <f t="shared" si="13"/>
-        <v>0.91901250000000012</v>
+        <v>1.2212654999999999</v>
       </c>
       <c r="T24" s="34">
         <f t="shared" si="13"/>
-        <v>0.48903749999999996</v>
+        <v>0.64987649999999997</v>
       </c>
       <c r="U24" s="34">
         <f t="shared" si="13"/>
-        <v>0.51975000000000005</v>
+        <v>0.69069000000000003</v>
       </c>
       <c r="V24" s="34">
         <f t="shared" si="13"/>
-        <v>2.7570375000000005</v>
+        <v>3.6637965000000006</v>
       </c>
       <c r="W24" s="34">
         <f t="shared" si="13"/>
-        <v>0.61897500000000005</v>
+        <v>0.82254899999999997</v>
       </c>
       <c r="X24" s="34">
         <f t="shared" si="13"/>
-        <v>1.6537500000000001</v>
+        <v>2.1976499999999999</v>
       </c>
       <c r="Y24" s="34">
         <f t="shared" si="13"/>
-        <v>0.96626250000000002</v>
+        <v>1.2840555</v>
       </c>
       <c r="Z24" s="34">
         <f t="shared" si="13"/>
-        <v>0.48903749999999996</v>
+        <v>0.64987649999999997</v>
       </c>
       <c r="AA24" s="34">
         <f t="shared" si="13"/>
-        <v>1.2922875</v>
+        <v>1.7173065000000001</v>
       </c>
       <c r="AB24" s="34">
         <f t="shared" si="13"/>
-        <v>0.17482500000000001</v>
+        <v>0.23232300000000003</v>
       </c>
       <c r="AC24" s="34">
         <f t="shared" si="13"/>
-        <v>0.61661250000000001</v>
+        <v>0.81940950000000001</v>
       </c>
       <c r="AD24" s="34">
         <f t="shared" si="13"/>
-        <v>0.34965000000000002</v>
+        <v>0.46464600000000006</v>
       </c>
       <c r="AE24" s="34">
         <f t="shared" si="13"/>
-        <v>0.48431249999999998</v>
+        <v>0.64359749999999993</v>
       </c>
       <c r="AF24" s="34">
         <f t="shared" si="13"/>
-        <v>0.43470000000000003</v>
+        <v>0.57766800000000007</v>
       </c>
       <c r="AG24" s="34">
         <f t="shared" si="13"/>
-        <v>0.75127500000000014</v>
+        <v>0.99836100000000005</v>
       </c>
       <c r="AH24" s="34">
         <f t="shared" si="13"/>
-        <v>0.60480000000000012</v>
+        <v>0.80371200000000009</v>
       </c>
       <c r="AI24" s="32"/>
     </row>
@@ -5433,112 +5433,112 @@
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="34">
-        <f>H21*3.4</f>
-        <v>39.394950000000001</v>
+        <f>H21*3.2</f>
+        <v>37.077600000000004</v>
       </c>
       <c r="I25" s="34">
-        <f t="shared" ref="I25:AH25" si="14">I21*3.4</f>
-        <v>0.52478999999999998</v>
+        <f t="shared" ref="I25:AH25" si="14">I21*3.2</f>
+        <v>0.49391999999999997</v>
       </c>
       <c r="J25" s="34">
         <f t="shared" si="14"/>
-        <v>10.588620000000001</v>
+        <v>9.9657600000000031</v>
       </c>
       <c r="K25" s="34">
         <f t="shared" si="14"/>
-        <v>1.9742100000000002</v>
+        <v>1.8580800000000004</v>
       </c>
       <c r="L25" s="34">
         <f t="shared" si="14"/>
-        <v>0.88893</v>
+        <v>0.83664000000000005</v>
       </c>
       <c r="M25" s="34">
         <f t="shared" si="14"/>
-        <v>0.77468999999999999</v>
+        <v>0.72911999999999999</v>
       </c>
       <c r="N25" s="34">
         <f t="shared" si="14"/>
-        <v>0.47838000000000003</v>
+        <v>0.45024000000000008</v>
       </c>
       <c r="O25" s="34">
         <f t="shared" si="14"/>
-        <v>1.3280399999999999</v>
+        <v>1.2499200000000001</v>
       </c>
       <c r="P25" s="34">
         <f t="shared" si="14"/>
-        <v>1.7100299999999999</v>
+        <v>1.6094400000000002</v>
       </c>
       <c r="Q25" s="34">
         <f t="shared" si="14"/>
-        <v>0.59262000000000004</v>
+        <v>0.55776000000000003</v>
       </c>
       <c r="R25" s="34">
         <f t="shared" si="14"/>
-        <v>0.70686000000000004</v>
+        <v>0.66528000000000009</v>
       </c>
       <c r="S25" s="34">
         <f t="shared" si="14"/>
-        <v>1.38873</v>
+        <v>1.3070400000000002</v>
       </c>
       <c r="T25" s="34">
         <f t="shared" si="14"/>
-        <v>0.73898999999999992</v>
+        <v>0.69552000000000003</v>
       </c>
       <c r="U25" s="34">
         <f t="shared" si="14"/>
-        <v>0.78539999999999999</v>
+        <v>0.73920000000000008</v>
       </c>
       <c r="V25" s="34">
         <f t="shared" si="14"/>
-        <v>4.1661900000000003</v>
+        <v>3.9211200000000006</v>
       </c>
       <c r="W25" s="34">
         <f t="shared" si="14"/>
-        <v>0.93534000000000006</v>
+        <v>0.8803200000000001</v>
       </c>
       <c r="X25" s="34">
         <f t="shared" si="14"/>
-        <v>2.4990000000000001</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="Y25" s="34">
         <f t="shared" si="14"/>
-        <v>1.4601299999999999</v>
+        <v>1.3742400000000001</v>
       </c>
       <c r="Z25" s="34">
         <f t="shared" si="14"/>
-        <v>0.73898999999999992</v>
+        <v>0.69552000000000003</v>
       </c>
       <c r="AA25" s="34">
         <f t="shared" si="14"/>
-        <v>1.95279</v>
+        <v>1.8379200000000002</v>
       </c>
       <c r="AB25" s="34">
         <f t="shared" si="14"/>
-        <v>0.26418000000000003</v>
+        <v>0.24864000000000003</v>
       </c>
       <c r="AC25" s="34">
         <f t="shared" si="14"/>
-        <v>0.93176999999999999</v>
+        <v>0.87696000000000007</v>
       </c>
       <c r="AD25" s="34">
         <f t="shared" si="14"/>
-        <v>0.52836000000000005</v>
+        <v>0.49728000000000006</v>
       </c>
       <c r="AE25" s="34">
         <f t="shared" si="14"/>
-        <v>0.73185</v>
+        <v>0.68880000000000008</v>
       </c>
       <c r="AF25" s="34">
         <f t="shared" si="14"/>
-        <v>0.65688000000000002</v>
+        <v>0.61824000000000012</v>
       </c>
       <c r="AG25" s="34">
         <f t="shared" si="14"/>
-        <v>1.1352600000000002</v>
+        <v>1.0684800000000001</v>
       </c>
       <c r="AH25" s="34">
         <f t="shared" si="14"/>
-        <v>0.91392000000000007</v>
+        <v>0.86016000000000015</v>
       </c>
       <c r="AI25" s="32"/>
     </row>
@@ -6566,7 +6566,10 @@
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
-      <c r="H36" s="34"/>
+      <c r="H36" s="34">
+        <f>H24-H23</f>
+        <v>19.581607499999997</v>
+      </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -6596,7 +6599,10 @@
       <c r="AI36" s="32"/>
     </row>
     <row r="37" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="26"/>
+      <c r="H37" s="26">
+        <f>H36/4</f>
+        <v>4.8954018749999992</v>
+      </c>
       <c r="I37" s="56"/>
       <c r="J37" s="26"/>
       <c r="K37" s="26"/>
@@ -6627,7 +6633,10 @@
     </row>
     <row r="38" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="52"/>
-      <c r="H38" s="26"/>
+      <c r="H38" s="26">
+        <f>H37+H23</f>
+        <v>19.958176874999999</v>
+      </c>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>

</xml_diff>

<commit_message>
Modify Max stock for MGT in 2070
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A010B85-ABAB-4381-826E-CDF63637366F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35D30E1-C547-46EF-ADA4-50093F0EF542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3202,8 +3202,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="Q11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25:AH25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5433,112 +5433,112 @@
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="34">
-        <f>H21*3.2</f>
-        <v>37.077600000000004</v>
+        <f>H21*3.4</f>
+        <v>39.394950000000001</v>
       </c>
       <c r="I25" s="34">
-        <f t="shared" ref="I25:AH25" si="14">I21*3.2</f>
-        <v>0.49391999999999997</v>
+        <f t="shared" ref="I25:AH25" si="14">I21*3.4</f>
+        <v>0.52478999999999998</v>
       </c>
       <c r="J25" s="34">
         <f t="shared" si="14"/>
-        <v>9.9657600000000031</v>
+        <v>10.588620000000001</v>
       </c>
       <c r="K25" s="34">
         <f t="shared" si="14"/>
-        <v>1.8580800000000004</v>
+        <v>1.9742100000000002</v>
       </c>
       <c r="L25" s="34">
         <f t="shared" si="14"/>
-        <v>0.83664000000000005</v>
+        <v>0.88893</v>
       </c>
       <c r="M25" s="34">
         <f t="shared" si="14"/>
-        <v>0.72911999999999999</v>
+        <v>0.77468999999999999</v>
       </c>
       <c r="N25" s="34">
         <f t="shared" si="14"/>
-        <v>0.45024000000000008</v>
+        <v>0.47838000000000003</v>
       </c>
       <c r="O25" s="34">
         <f t="shared" si="14"/>
-        <v>1.2499200000000001</v>
+        <v>1.3280399999999999</v>
       </c>
       <c r="P25" s="34">
         <f t="shared" si="14"/>
-        <v>1.6094400000000002</v>
+        <v>1.7100299999999999</v>
       </c>
       <c r="Q25" s="34">
         <f t="shared" si="14"/>
-        <v>0.55776000000000003</v>
+        <v>0.59262000000000004</v>
       </c>
       <c r="R25" s="34">
         <f t="shared" si="14"/>
-        <v>0.66528000000000009</v>
+        <v>0.70686000000000004</v>
       </c>
       <c r="S25" s="34">
         <f t="shared" si="14"/>
-        <v>1.3070400000000002</v>
+        <v>1.38873</v>
       </c>
       <c r="T25" s="34">
         <f t="shared" si="14"/>
-        <v>0.69552000000000003</v>
+        <v>0.73898999999999992</v>
       </c>
       <c r="U25" s="34">
         <f t="shared" si="14"/>
-        <v>0.73920000000000008</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="V25" s="34">
         <f t="shared" si="14"/>
-        <v>3.9211200000000006</v>
+        <v>4.1661900000000003</v>
       </c>
       <c r="W25" s="34">
         <f t="shared" si="14"/>
-        <v>0.8803200000000001</v>
+        <v>0.93534000000000006</v>
       </c>
       <c r="X25" s="34">
         <f t="shared" si="14"/>
-        <v>2.3519999999999999</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="Y25" s="34">
         <f t="shared" si="14"/>
-        <v>1.3742400000000001</v>
+        <v>1.4601299999999999</v>
       </c>
       <c r="Z25" s="34">
         <f t="shared" si="14"/>
-        <v>0.69552000000000003</v>
+        <v>0.73898999999999992</v>
       </c>
       <c r="AA25" s="34">
         <f t="shared" si="14"/>
-        <v>1.8379200000000002</v>
+        <v>1.95279</v>
       </c>
       <c r="AB25" s="34">
         <f t="shared" si="14"/>
-        <v>0.24864000000000003</v>
+        <v>0.26418000000000003</v>
       </c>
       <c r="AC25" s="34">
         <f t="shared" si="14"/>
-        <v>0.87696000000000007</v>
+        <v>0.93176999999999999</v>
       </c>
       <c r="AD25" s="34">
         <f t="shared" si="14"/>
-        <v>0.49728000000000006</v>
+        <v>0.52836000000000005</v>
       </c>
       <c r="AE25" s="34">
         <f t="shared" si="14"/>
-        <v>0.68880000000000008</v>
+        <v>0.73185</v>
       </c>
       <c r="AF25" s="34">
         <f t="shared" si="14"/>
-        <v>0.61824000000000012</v>
+        <v>0.65688000000000002</v>
       </c>
       <c r="AG25" s="34">
         <f t="shared" si="14"/>
-        <v>1.0684800000000001</v>
+        <v>1.1352600000000002</v>
       </c>
       <c r="AH25" s="34">
         <f t="shared" si="14"/>
-        <v>0.86016000000000015</v>
+        <v>0.91392000000000007</v>
       </c>
       <c r="AI25" s="32"/>
     </row>

</xml_diff>

<commit_message>
Increase max stock for HGTs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35D30E1-C547-46EF-ADA4-50093F0EF542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E141F-9CA2-43DA-9D3C-B6098A24960F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,9 +597,6 @@
     <t>Stock in 2018</t>
   </si>
   <si>
-    <t>STOCK in 2018</t>
-  </si>
-  <si>
     <t>UC_MGT_Stock</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   <si>
     <t>~UC_T:UC_RHSRTS</t>
   </si>
+  <si>
+    <t>STOCK in 2018 (kunit)</t>
+  </si>
 </sst>
 </file>
 
@@ -634,7 +634,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="42" x14ac:knownFonts="1">
     <font>
@@ -1464,7 +1464,7 @@
     <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1537,15 +1537,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="41" fillId="43" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="68" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="68" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="20% - Accent1" xfId="45" builtinId="30" customBuiltin="1"/>
@@ -3202,8 +3204,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:AH25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3236,9 +3238,9 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI5" s="51"/>
+        <v>143</v>
+      </c>
+      <c r="AI5" s="50"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
@@ -3367,7 +3369,7 @@
         <f>Regions!AD$3</f>
         <v>IE-MN</v>
       </c>
-      <c r="AI6" s="51"/>
+      <c r="AI6" s="50"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -3382,460 +3384,460 @@
       <c r="G7" t="s">
         <v>97</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="55">
         <f>H42*1.05</f>
         <v>2228.8843500000003</v>
       </c>
-      <c r="I7" s="57">
+      <c r="I7" s="55">
         <f t="shared" ref="I7:AH7" si="0">I42*1.05</f>
         <v>29.98695</v>
       </c>
-      <c r="J7" s="57">
+      <c r="J7" s="55">
         <f t="shared" si="0"/>
         <v>554.76225000000022</v>
       </c>
-      <c r="K7" s="57">
+      <c r="K7" s="55">
         <f t="shared" si="0"/>
         <v>107.68275000000003</v>
       </c>
-      <c r="L7" s="57">
+      <c r="L7" s="55">
         <f t="shared" si="0"/>
         <v>48.583499999999994</v>
       </c>
-      <c r="M7" s="57">
+      <c r="M7" s="55">
         <f t="shared" si="0"/>
         <v>36.785699999999999</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="55">
         <f t="shared" si="0"/>
         <v>19.214999999999996</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="55">
         <f t="shared" si="0"/>
         <v>53.548949999999998</v>
       </c>
-      <c r="P7" s="57">
+      <c r="P7" s="55">
         <f t="shared" si="0"/>
         <v>91.8309</v>
       </c>
-      <c r="Q7" s="57">
+      <c r="Q7" s="55">
         <f t="shared" si="0"/>
         <v>36.018149999999999</v>
       </c>
-      <c r="R7" s="57">
+      <c r="R7" s="55">
         <f t="shared" si="0"/>
         <v>43.430099999999996</v>
       </c>
-      <c r="S7" s="57">
+      <c r="S7" s="55">
         <f t="shared" si="0"/>
         <v>78.821400000000011</v>
       </c>
-      <c r="T7" s="57">
+      <c r="T7" s="55">
         <f t="shared" si="0"/>
         <v>71.70975</v>
       </c>
-      <c r="U7" s="57">
+      <c r="U7" s="55">
         <f t="shared" si="0"/>
         <v>60.372900000000001</v>
       </c>
-      <c r="V7" s="57">
+      <c r="V7" s="55">
         <f t="shared" si="0"/>
         <v>271.39140000000003</v>
       </c>
-      <c r="W7" s="57">
+      <c r="W7" s="55">
         <f t="shared" si="0"/>
         <v>76.935599999999994</v>
       </c>
-      <c r="X7" s="57">
+      <c r="X7" s="55">
         <f t="shared" si="0"/>
         <v>92.664599999999993</v>
       </c>
-      <c r="Y7" s="57">
+      <c r="Y7" s="55">
         <f t="shared" si="0"/>
         <v>82.989900000000006</v>
       </c>
-      <c r="Z7" s="57">
+      <c r="Z7" s="55">
         <f t="shared" si="0"/>
         <v>60.668999999999997</v>
       </c>
-      <c r="AA7" s="57">
+      <c r="AA7" s="55">
         <f t="shared" si="0"/>
         <v>136.81920000000005</v>
       </c>
-      <c r="AB7" s="57">
+      <c r="AB7" s="55">
         <f t="shared" si="0"/>
         <v>15.622949999999999</v>
       </c>
-      <c r="AC7" s="57">
+      <c r="AC7" s="55">
         <f t="shared" si="0"/>
         <v>64.41749999999999</v>
       </c>
-      <c r="AD7" s="57">
+      <c r="AD7" s="55">
         <f t="shared" si="0"/>
         <v>34.345500000000008</v>
       </c>
-      <c r="AE7" s="57">
+      <c r="AE7" s="55">
         <f t="shared" si="0"/>
         <v>30.602249999999998</v>
       </c>
-      <c r="AF7" s="57">
+      <c r="AF7" s="55">
         <f t="shared" si="0"/>
         <v>33.474000000000004</v>
       </c>
-      <c r="AG7" s="57">
+      <c r="AG7" s="55">
         <f t="shared" si="0"/>
         <v>67.603200000000015</v>
       </c>
-      <c r="AH7" s="57">
+      <c r="AH7" s="55">
         <f t="shared" si="0"/>
         <v>28.600950000000005</v>
       </c>
-      <c r="AI7" s="51"/>
-    </row>
-    <row r="8" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AI7" s="50"/>
+    </row>
+    <row r="8" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E8" s="30">
         <v>2022</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="55">
         <f>H7*1.01</f>
         <v>2251.1731935000003</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="55">
         <f t="shared" ref="I8:AH8" si="1">I7*1.01</f>
         <v>30.2868195</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J8" s="55">
         <f t="shared" si="1"/>
         <v>560.30987250000021</v>
       </c>
-      <c r="K8" s="57">
+      <c r="K8" s="55">
         <f t="shared" si="1"/>
         <v>108.75957750000003</v>
       </c>
-      <c r="L8" s="57">
+      <c r="L8" s="55">
         <f t="shared" si="1"/>
         <v>49.069334999999995</v>
       </c>
-      <c r="M8" s="57">
+      <c r="M8" s="55">
         <f t="shared" si="1"/>
         <v>37.153556999999999</v>
       </c>
-      <c r="N8" s="57">
+      <c r="N8" s="55">
         <f t="shared" si="1"/>
         <v>19.407149999999998</v>
       </c>
-      <c r="O8" s="57">
+      <c r="O8" s="55">
         <f t="shared" si="1"/>
         <v>54.084439499999995</v>
       </c>
-      <c r="P8" s="57">
+      <c r="P8" s="55">
         <f t="shared" si="1"/>
         <v>92.749209000000008</v>
       </c>
-      <c r="Q8" s="57">
+      <c r="Q8" s="55">
         <f t="shared" si="1"/>
         <v>36.378331500000002</v>
       </c>
-      <c r="R8" s="57">
+      <c r="R8" s="55">
         <f t="shared" si="1"/>
         <v>43.864400999999994</v>
       </c>
-      <c r="S8" s="57">
+      <c r="S8" s="55">
         <f t="shared" si="1"/>
         <v>79.609614000000008</v>
       </c>
-      <c r="T8" s="57">
+      <c r="T8" s="55">
         <f t="shared" si="1"/>
         <v>72.426847499999994</v>
       </c>
-      <c r="U8" s="57">
+      <c r="U8" s="55">
         <f t="shared" si="1"/>
         <v>60.976629000000003</v>
       </c>
-      <c r="V8" s="57">
+      <c r="V8" s="55">
         <f t="shared" si="1"/>
         <v>274.10531400000002</v>
       </c>
-      <c r="W8" s="57">
+      <c r="W8" s="55">
         <f t="shared" si="1"/>
         <v>77.704955999999996</v>
       </c>
-      <c r="X8" s="57">
+      <c r="X8" s="55">
         <f t="shared" si="1"/>
         <v>93.591245999999998</v>
       </c>
-      <c r="Y8" s="57">
+      <c r="Y8" s="55">
         <f t="shared" si="1"/>
         <v>83.819799000000003</v>
       </c>
-      <c r="Z8" s="57">
+      <c r="Z8" s="55">
         <f t="shared" si="1"/>
         <v>61.275689999999997</v>
       </c>
-      <c r="AA8" s="57">
+      <c r="AA8" s="55">
         <f t="shared" si="1"/>
         <v>138.18739200000005</v>
       </c>
-      <c r="AB8" s="57">
+      <c r="AB8" s="55">
         <f t="shared" si="1"/>
         <v>15.7791795</v>
       </c>
-      <c r="AC8" s="57">
+      <c r="AC8" s="55">
         <f t="shared" si="1"/>
         <v>65.061674999999994</v>
       </c>
-      <c r="AD8" s="57">
+      <c r="AD8" s="55">
         <f t="shared" si="1"/>
         <v>34.688955000000007</v>
       </c>
-      <c r="AE8" s="57">
+      <c r="AE8" s="55">
         <f t="shared" si="1"/>
         <v>30.908272499999999</v>
       </c>
-      <c r="AF8" s="57">
+      <c r="AF8" s="55">
         <f t="shared" si="1"/>
         <v>33.808740000000007</v>
       </c>
-      <c r="AG8" s="57">
+      <c r="AG8" s="55">
         <f t="shared" si="1"/>
         <v>68.279232000000022</v>
       </c>
-      <c r="AH8" s="57">
+      <c r="AH8" s="55">
         <f t="shared" si="1"/>
         <v>28.886959500000003</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E9" s="30">
         <v>2030</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="55">
         <f>H8*1.05</f>
         <v>2363.7318531750002</v>
       </c>
-      <c r="I9" s="57">
+      <c r="I9" s="55">
         <f t="shared" ref="I9:AH9" si="2">I8*1.05</f>
         <v>31.801160475</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="55">
         <f t="shared" si="2"/>
         <v>588.3253661250003</v>
       </c>
-      <c r="K9" s="57">
+      <c r="K9" s="55">
         <f t="shared" si="2"/>
         <v>114.19755637500005</v>
       </c>
-      <c r="L9" s="57">
+      <c r="L9" s="55">
         <f t="shared" si="2"/>
         <v>51.522801749999999</v>
       </c>
-      <c r="M9" s="57">
+      <c r="M9" s="55">
         <f t="shared" si="2"/>
         <v>39.011234850000001</v>
       </c>
-      <c r="N9" s="57">
+      <c r="N9" s="55">
         <f t="shared" si="2"/>
         <v>20.3775075</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="55">
         <f t="shared" si="2"/>
         <v>56.788661474999998</v>
       </c>
-      <c r="P9" s="57">
+      <c r="P9" s="55">
         <f t="shared" si="2"/>
         <v>97.386669450000014</v>
       </c>
-      <c r="Q9" s="57">
+      <c r="Q9" s="55">
         <f t="shared" si="2"/>
         <v>38.197248075000005</v>
       </c>
-      <c r="R9" s="57">
+      <c r="R9" s="55">
         <f t="shared" si="2"/>
         <v>46.057621049999995</v>
       </c>
-      <c r="S9" s="57">
+      <c r="S9" s="55">
         <f t="shared" si="2"/>
         <v>83.590094700000009</v>
       </c>
-      <c r="T9" s="57">
+      <c r="T9" s="55">
         <f t="shared" si="2"/>
         <v>76.048189874999991</v>
       </c>
-      <c r="U9" s="57">
+      <c r="U9" s="55">
         <f t="shared" si="2"/>
         <v>64.025460450000011</v>
       </c>
-      <c r="V9" s="57">
+      <c r="V9" s="55">
         <f t="shared" si="2"/>
         <v>287.81057970000006</v>
       </c>
-      <c r="W9" s="57">
+      <c r="W9" s="55">
         <f t="shared" si="2"/>
         <v>81.590203799999998</v>
       </c>
-      <c r="X9" s="57">
+      <c r="X9" s="55">
         <f t="shared" si="2"/>
         <v>98.270808299999999</v>
       </c>
-      <c r="Y9" s="57">
+      <c r="Y9" s="55">
         <f t="shared" si="2"/>
         <v>88.010788950000006</v>
       </c>
-      <c r="Z9" s="57">
+      <c r="Z9" s="55">
         <f t="shared" si="2"/>
         <v>64.339474499999994</v>
       </c>
-      <c r="AA9" s="57">
+      <c r="AA9" s="55">
         <f t="shared" si="2"/>
         <v>145.09676160000006</v>
       </c>
-      <c r="AB9" s="57">
+      <c r="AB9" s="55">
         <f t="shared" si="2"/>
         <v>16.568138475000001</v>
       </c>
-      <c r="AC9" s="57">
+      <c r="AC9" s="55">
         <f t="shared" si="2"/>
         <v>68.314758749999996</v>
       </c>
-      <c r="AD9" s="57">
+      <c r="AD9" s="55">
         <f t="shared" si="2"/>
         <v>36.423402750000008</v>
       </c>
-      <c r="AE9" s="57">
+      <c r="AE9" s="55">
         <f t="shared" si="2"/>
         <v>32.453686124999997</v>
       </c>
-      <c r="AF9" s="57">
+      <c r="AF9" s="55">
         <f t="shared" si="2"/>
         <v>35.49917700000001</v>
       </c>
-      <c r="AG9" s="57">
+      <c r="AG9" s="55">
         <f t="shared" si="2"/>
         <v>71.693193600000029</v>
       </c>
-      <c r="AH9" s="57">
+      <c r="AH9" s="55">
         <f t="shared" si="2"/>
         <v>30.331307475000006</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E10" s="30">
         <v>2050</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="55">
         <f>H9*1.12</f>
         <v>2647.3796755560006</v>
       </c>
-      <c r="I10" s="57">
+      <c r="I10" s="55">
         <f t="shared" ref="I10:AH10" si="3">I9*1.12</f>
         <v>35.617299732000006</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="55">
         <f t="shared" si="3"/>
         <v>658.92441006000035</v>
       </c>
-      <c r="K10" s="57">
+      <c r="K10" s="55">
         <f t="shared" si="3"/>
         <v>127.90126314000007</v>
       </c>
-      <c r="L10" s="57">
+      <c r="L10" s="55">
         <f t="shared" si="3"/>
         <v>57.705537960000008</v>
       </c>
-      <c r="M10" s="57">
+      <c r="M10" s="55">
         <f t="shared" si="3"/>
         <v>43.692583032000009</v>
       </c>
-      <c r="N10" s="57">
+      <c r="N10" s="55">
         <f t="shared" si="3"/>
         <v>22.822808400000003</v>
       </c>
-      <c r="O10" s="57">
+      <c r="O10" s="55">
         <f t="shared" si="3"/>
         <v>63.603300852000004</v>
       </c>
-      <c r="P10" s="57">
+      <c r="P10" s="55">
         <f t="shared" si="3"/>
         <v>109.07306978400003</v>
       </c>
-      <c r="Q10" s="57">
+      <c r="Q10" s="55">
         <f t="shared" si="3"/>
         <v>42.780917844000008</v>
       </c>
-      <c r="R10" s="57">
+      <c r="R10" s="55">
         <f t="shared" si="3"/>
         <v>51.584535576</v>
       </c>
-      <c r="S10" s="57">
+      <c r="S10" s="55">
         <f t="shared" si="3"/>
         <v>93.620906064000025</v>
       </c>
-      <c r="T10" s="57">
+      <c r="T10" s="55">
         <f t="shared" si="3"/>
         <v>85.173972660000004</v>
       </c>
-      <c r="U10" s="57">
+      <c r="U10" s="55">
         <f t="shared" si="3"/>
         <v>71.708515704000021</v>
       </c>
-      <c r="V10" s="57">
+      <c r="V10" s="55">
         <f t="shared" si="3"/>
         <v>322.3478492640001</v>
       </c>
-      <c r="W10" s="57">
+      <c r="W10" s="55">
         <f t="shared" si="3"/>
         <v>91.381028256000008</v>
       </c>
-      <c r="X10" s="57">
+      <c r="X10" s="55">
         <f t="shared" si="3"/>
         <v>110.06330529600001</v>
       </c>
-      <c r="Y10" s="57">
+      <c r="Y10" s="55">
         <f t="shared" si="3"/>
         <v>98.572083624000015</v>
       </c>
-      <c r="Z10" s="57">
+      <c r="Z10" s="55">
         <f t="shared" si="3"/>
         <v>72.060211440000003</v>
       </c>
-      <c r="AA10" s="57">
+      <c r="AA10" s="55">
         <f t="shared" si="3"/>
         <v>162.50837299200009</v>
       </c>
-      <c r="AB10" s="57">
+      <c r="AB10" s="55">
         <f t="shared" si="3"/>
         <v>18.556315092000002</v>
       </c>
-      <c r="AC10" s="57">
+      <c r="AC10" s="55">
         <f t="shared" si="3"/>
         <v>76.512529799999996</v>
       </c>
-      <c r="AD10" s="57">
+      <c r="AD10" s="55">
         <f t="shared" si="3"/>
         <v>40.794211080000011</v>
       </c>
-      <c r="AE10" s="57">
+      <c r="AE10" s="55">
         <f t="shared" si="3"/>
         <v>36.348128459999998</v>
       </c>
-      <c r="AF10" s="57">
+      <c r="AF10" s="55">
         <f t="shared" si="3"/>
         <v>39.759078240000015</v>
       </c>
-      <c r="AG10" s="57">
+      <c r="AG10" s="55">
         <f t="shared" si="3"/>
         <v>80.296376832000036</v>
       </c>
-      <c r="AH10" s="57">
+      <c r="AH10" s="55">
         <f t="shared" si="3"/>
         <v>33.971064372000008</v>
       </c>
@@ -3844,118 +3846,118 @@
       <c r="E11" s="30">
         <v>2070</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="55">
         <f>H7*1.35</f>
         <v>3008.9938725000006</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="55">
         <f t="shared" ref="I11:AH11" si="4">I7*1.35</f>
         <v>40.4823825</v>
       </c>
-      <c r="J11" s="57">
+      <c r="J11" s="55">
         <f t="shared" si="4"/>
         <v>748.92903750000039</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="55">
         <f t="shared" si="4"/>
         <v>145.37171250000006</v>
       </c>
-      <c r="L11" s="57">
+      <c r="L11" s="55">
         <f t="shared" si="4"/>
         <v>65.587724999999992</v>
       </c>
-      <c r="M11" s="57">
+      <c r="M11" s="55">
         <f t="shared" si="4"/>
         <v>49.660695000000004</v>
       </c>
-      <c r="N11" s="57">
+      <c r="N11" s="55">
         <f t="shared" si="4"/>
         <v>25.940249999999995</v>
       </c>
-      <c r="O11" s="57">
+      <c r="O11" s="55">
         <f t="shared" si="4"/>
         <v>72.291082500000002</v>
       </c>
-      <c r="P11" s="57">
+      <c r="P11" s="55">
         <f t="shared" si="4"/>
         <v>123.971715</v>
       </c>
-      <c r="Q11" s="57">
+      <c r="Q11" s="55">
         <f t="shared" si="4"/>
         <v>48.624502499999998</v>
       </c>
-      <c r="R11" s="57">
+      <c r="R11" s="55">
         <f t="shared" si="4"/>
         <v>58.630634999999998</v>
       </c>
-      <c r="S11" s="57">
+      <c r="S11" s="55">
         <f t="shared" si="4"/>
         <v>106.40889000000003</v>
       </c>
-      <c r="T11" s="57">
+      <c r="T11" s="55">
         <f t="shared" si="4"/>
         <v>96.808162500000009</v>
       </c>
-      <c r="U11" s="57">
+      <c r="U11" s="55">
         <f t="shared" si="4"/>
         <v>81.503415000000004</v>
       </c>
-      <c r="V11" s="57">
+      <c r="V11" s="55">
         <f t="shared" si="4"/>
         <v>366.37839000000008</v>
       </c>
-      <c r="W11" s="57">
+      <c r="W11" s="55">
         <f t="shared" si="4"/>
         <v>103.86306</v>
       </c>
-      <c r="X11" s="57">
+      <c r="X11" s="55">
         <f t="shared" si="4"/>
         <v>125.09721</v>
       </c>
-      <c r="Y11" s="57">
+      <c r="Y11" s="55">
         <f t="shared" si="4"/>
         <v>112.03636500000002</v>
       </c>
-      <c r="Z11" s="57">
+      <c r="Z11" s="55">
         <f t="shared" si="4"/>
         <v>81.903149999999997</v>
       </c>
-      <c r="AA11" s="57">
+      <c r="AA11" s="55">
         <f t="shared" si="4"/>
         <v>184.70592000000008</v>
       </c>
-      <c r="AB11" s="57">
+      <c r="AB11" s="55">
         <f t="shared" si="4"/>
         <v>21.090982499999999</v>
       </c>
-      <c r="AC11" s="57">
+      <c r="AC11" s="55">
         <f t="shared" si="4"/>
         <v>86.963624999999993</v>
       </c>
-      <c r="AD11" s="57">
+      <c r="AD11" s="55">
         <f t="shared" si="4"/>
         <v>46.366425000000014</v>
       </c>
-      <c r="AE11" s="57">
+      <c r="AE11" s="55">
         <f t="shared" si="4"/>
         <v>41.3130375</v>
       </c>
-      <c r="AF11" s="57">
+      <c r="AF11" s="55">
         <f t="shared" si="4"/>
         <v>45.189900000000009</v>
       </c>
-      <c r="AG11" s="57">
+      <c r="AG11" s="55">
         <f t="shared" si="4"/>
         <v>91.264320000000026</v>
       </c>
-      <c r="AH11" s="57">
+      <c r="AH11" s="55">
         <f t="shared" si="4"/>
         <v>38.611282500000009</v>
       </c>
-      <c r="AI11" s="51"/>
+      <c r="AI11" s="50"/>
     </row>
     <row r="12" spans="1:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32"/>
@@ -3963,94 +3965,94 @@
       <c r="E12" s="33">
         <v>0</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G12" s="32"/>
-      <c r="H12" s="53">
+      <c r="H12" s="52">
         <v>5</v>
       </c>
-      <c r="I12" s="53">
+      <c r="I12" s="52">
         <v>5</v>
       </c>
-      <c r="J12" s="53">
+      <c r="J12" s="52">
         <v>5</v>
       </c>
-      <c r="K12" s="53">
+      <c r="K12" s="52">
         <v>5</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="52">
         <v>5</v>
       </c>
-      <c r="M12" s="53">
+      <c r="M12" s="52">
         <v>5</v>
       </c>
-      <c r="N12" s="53">
+      <c r="N12" s="52">
         <v>5</v>
       </c>
-      <c r="O12" s="53">
+      <c r="O12" s="52">
         <v>5</v>
       </c>
-      <c r="P12" s="53">
+      <c r="P12" s="52">
         <v>5</v>
       </c>
-      <c r="Q12" s="53">
+      <c r="Q12" s="52">
         <v>5</v>
       </c>
-      <c r="R12" s="53">
+      <c r="R12" s="52">
         <v>5</v>
       </c>
-      <c r="S12" s="53">
+      <c r="S12" s="52">
         <v>5</v>
       </c>
-      <c r="T12" s="53">
+      <c r="T12" s="52">
         <v>5</v>
       </c>
-      <c r="U12" s="53">
+      <c r="U12" s="52">
         <v>5</v>
       </c>
-      <c r="V12" s="53">
+      <c r="V12" s="52">
         <v>5</v>
       </c>
-      <c r="W12" s="53">
+      <c r="W12" s="52">
         <v>5</v>
       </c>
-      <c r="X12" s="53">
+      <c r="X12" s="52">
         <v>5</v>
       </c>
-      <c r="Y12" s="53">
+      <c r="Y12" s="52">
         <v>5</v>
       </c>
-      <c r="Z12" s="53">
+      <c r="Z12" s="52">
         <v>5</v>
       </c>
-      <c r="AA12" s="53">
+      <c r="AA12" s="52">
         <v>5</v>
       </c>
-      <c r="AB12" s="53">
+      <c r="AB12" s="52">
         <v>5</v>
       </c>
-      <c r="AC12" s="53">
+      <c r="AC12" s="52">
         <v>5</v>
       </c>
-      <c r="AD12" s="53">
+      <c r="AD12" s="52">
         <v>5</v>
       </c>
-      <c r="AE12" s="53">
+      <c r="AE12" s="52">
         <v>5</v>
       </c>
-      <c r="AF12" s="53">
+      <c r="AF12" s="52">
         <v>5</v>
       </c>
-      <c r="AG12" s="53">
+      <c r="AG12" s="52">
         <v>5</v>
       </c>
-      <c r="AH12" s="53">
+      <c r="AH12" s="52">
         <v>5</v>
       </c>
       <c r="AI12" s="32"/>
     </row>
-    <row r="13" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="29"/>
       <c r="C13" s="29" t="s">
         <v>102</v>
@@ -4061,87 +4063,87 @@
       <c r="E13" s="31">
         <v>2018</v>
       </c>
-      <c r="F13" s="55"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="54">
+      <c r="H13" s="53">
         <v>1</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="53">
         <v>1</v>
       </c>
-      <c r="J13" s="54">
+      <c r="J13" s="53">
         <v>1</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K13" s="53">
         <v>1</v>
       </c>
-      <c r="L13" s="54">
+      <c r="L13" s="53">
         <v>1</v>
       </c>
-      <c r="M13" s="54">
+      <c r="M13" s="53">
         <v>1</v>
       </c>
-      <c r="N13" s="54">
+      <c r="N13" s="53">
         <v>1</v>
       </c>
-      <c r="O13" s="54">
+      <c r="O13" s="53">
         <v>1</v>
       </c>
-      <c r="P13" s="54">
+      <c r="P13" s="53">
         <v>1</v>
       </c>
-      <c r="Q13" s="54">
+      <c r="Q13" s="53">
         <v>1</v>
       </c>
-      <c r="R13" s="54">
+      <c r="R13" s="53">
         <v>1</v>
       </c>
-      <c r="S13" s="54">
+      <c r="S13" s="53">
         <v>1</v>
       </c>
-      <c r="T13" s="54">
+      <c r="T13" s="53">
         <v>1</v>
       </c>
-      <c r="U13" s="54">
+      <c r="U13" s="53">
         <v>1</v>
       </c>
-      <c r="V13" s="54">
+      <c r="V13" s="53">
         <v>1</v>
       </c>
-      <c r="W13" s="54">
+      <c r="W13" s="53">
         <v>1</v>
       </c>
-      <c r="X13" s="54">
+      <c r="X13" s="53">
         <v>1</v>
       </c>
-      <c r="Y13" s="54">
+      <c r="Y13" s="53">
         <v>1</v>
       </c>
-      <c r="Z13" s="54">
+      <c r="Z13" s="53">
         <v>1</v>
       </c>
-      <c r="AA13" s="54">
+      <c r="AA13" s="53">
         <v>1</v>
       </c>
-      <c r="AB13" s="54">
+      <c r="AB13" s="53">
         <v>1</v>
       </c>
-      <c r="AC13" s="54">
+      <c r="AC13" s="53">
         <v>1</v>
       </c>
-      <c r="AD13" s="54">
+      <c r="AD13" s="53">
         <v>1</v>
       </c>
-      <c r="AE13" s="54">
+      <c r="AE13" s="53">
         <v>1</v>
       </c>
-      <c r="AF13" s="54">
+      <c r="AF13" s="53">
         <v>1</v>
       </c>
-      <c r="AG13" s="54">
+      <c r="AG13" s="53">
         <v>1</v>
       </c>
-      <c r="AH13" s="54">
+      <c r="AH13" s="53">
         <v>1</v>
       </c>
       <c r="AI13" s="32"/>
@@ -4150,12 +4152,12 @@
       <c r="B14" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="30">
         <v>2018</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G14" s="32" t="s">
@@ -4271,358 +4273,358 @@
       </c>
       <c r="AI14" s="32"/>
     </row>
-    <row r="15" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="32"/>
       <c r="E15" s="30">
         <v>2022</v>
       </c>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G15" s="32"/>
-      <c r="H15" s="34">
+      <c r="H15" s="52">
         <f>H14*1.1</f>
         <v>371.64781500000004</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="52">
         <f t="shared" ref="I15:AH15" si="6">I14*1.1</f>
         <v>6.0891599999999997</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="52">
         <f t="shared" si="6"/>
         <v>78.163470000000018</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="52">
         <f t="shared" si="6"/>
         <v>16.662030000000001</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="52">
         <f t="shared" si="6"/>
         <v>8.3841450000000002</v>
       </c>
-      <c r="M15" s="34">
+      <c r="M15" s="52">
         <f t="shared" si="6"/>
         <v>6.1931100000000008</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N15" s="52">
         <f t="shared" si="6"/>
         <v>4.0759949999999998</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="52">
         <f t="shared" si="6"/>
         <v>8.2628700000000013</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="52">
         <f t="shared" si="6"/>
         <v>14.877555000000001</v>
       </c>
-      <c r="Q15" s="34">
+      <c r="Q15" s="52">
         <f t="shared" si="6"/>
         <v>6.9727350000000001</v>
       </c>
-      <c r="R15" s="34">
+      <c r="R15" s="52">
         <f t="shared" si="6"/>
         <v>8.7722250000000024</v>
       </c>
-      <c r="S15" s="34">
+      <c r="S15" s="52">
         <f t="shared" si="6"/>
         <v>14.101395</v>
       </c>
-      <c r="T15" s="34">
+      <c r="T15" s="52">
         <f t="shared" si="6"/>
         <v>10.202115000000003</v>
       </c>
-      <c r="U15" s="34">
+      <c r="U15" s="52">
         <f t="shared" si="6"/>
         <v>10.184790000000001</v>
       </c>
-      <c r="V15" s="34">
+      <c r="V15" s="52">
         <f t="shared" si="6"/>
         <v>43.656690000000012</v>
       </c>
-      <c r="W15" s="34">
+      <c r="W15" s="52">
         <f t="shared" si="6"/>
         <v>12.867855</v>
       </c>
-      <c r="X15" s="34">
+      <c r="X15" s="52">
         <f t="shared" si="6"/>
         <v>13.868085000000001</v>
       </c>
-      <c r="Y15" s="34">
+      <c r="Y15" s="52">
         <f t="shared" si="6"/>
         <v>14.440965000000002</v>
       </c>
-      <c r="Z15" s="34">
+      <c r="Z15" s="52">
         <f t="shared" si="6"/>
         <v>8.774535000000002</v>
       </c>
-      <c r="AA15" s="34">
+      <c r="AA15" s="52">
         <f t="shared" si="6"/>
         <v>21.695519999999998</v>
       </c>
-      <c r="AB15" s="34">
+      <c r="AB15" s="52">
         <f t="shared" si="6"/>
         <v>3.6902250000000003</v>
       </c>
-      <c r="AC15" s="34">
+      <c r="AC15" s="52">
         <f t="shared" si="6"/>
         <v>14.472150000000001</v>
       </c>
-      <c r="AD15" s="34">
+      <c r="AD15" s="52">
         <f t="shared" si="6"/>
         <v>6.8260500000000013</v>
       </c>
-      <c r="AE15" s="34">
+      <c r="AE15" s="52">
         <f t="shared" si="6"/>
         <v>6.4783950000000008</v>
       </c>
-      <c r="AF15" s="34">
+      <c r="AF15" s="52">
         <f t="shared" si="6"/>
         <v>8.5204350000000009</v>
       </c>
-      <c r="AG15" s="34">
+      <c r="AG15" s="52">
         <f t="shared" si="6"/>
         <v>15.704535000000002</v>
       </c>
-      <c r="AH15" s="34">
+      <c r="AH15" s="52">
         <f t="shared" si="6"/>
         <v>7.7107799999999997</v>
       </c>
       <c r="AI15" s="32"/>
     </row>
-    <row r="16" spans="1:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="32"/>
       <c r="E16" s="30">
         <v>2030</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G16" s="32"/>
-      <c r="H16" s="34">
+      <c r="H16" s="52">
         <f>H15*1.09</f>
         <v>405.0961183500001</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="52">
         <f t="shared" ref="I16:AH16" si="7">I15*1.09</f>
         <v>6.6371843999999998</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="52">
         <f t="shared" si="7"/>
         <v>85.198182300000028</v>
       </c>
-      <c r="K16" s="34">
+      <c r="K16" s="52">
         <f t="shared" si="7"/>
         <v>18.161612700000003</v>
       </c>
-      <c r="L16" s="34">
+      <c r="L16" s="52">
         <f t="shared" si="7"/>
         <v>9.1387180500000014</v>
       </c>
-      <c r="M16" s="34">
+      <c r="M16" s="52">
         <f t="shared" si="7"/>
         <v>6.7504899000000016</v>
       </c>
-      <c r="N16" s="34">
+      <c r="N16" s="52">
         <f t="shared" si="7"/>
         <v>4.4428345499999997</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="52">
         <f t="shared" si="7"/>
         <v>9.0065283000000029</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="52">
         <f t="shared" si="7"/>
         <v>16.216534950000003</v>
       </c>
-      <c r="Q16" s="34">
+      <c r="Q16" s="52">
         <f t="shared" si="7"/>
         <v>7.6002811500000007</v>
       </c>
-      <c r="R16" s="34">
+      <c r="R16" s="52">
         <f t="shared" si="7"/>
         <v>9.5617252500000038</v>
       </c>
-      <c r="S16" s="34">
+      <c r="S16" s="52">
         <f t="shared" si="7"/>
         <v>15.370520550000002</v>
       </c>
-      <c r="T16" s="34">
+      <c r="T16" s="52">
         <f t="shared" si="7"/>
         <v>11.120305350000004</v>
       </c>
-      <c r="U16" s="34">
+      <c r="U16" s="52">
         <f t="shared" si="7"/>
         <v>11.101421100000003</v>
       </c>
-      <c r="V16" s="34">
+      <c r="V16" s="52">
         <f t="shared" si="7"/>
         <v>47.585792100000013</v>
       </c>
-      <c r="W16" s="34">
+      <c r="W16" s="52">
         <f t="shared" si="7"/>
         <v>14.025961950000001</v>
       </c>
-      <c r="X16" s="34">
+      <c r="X16" s="52">
         <f t="shared" si="7"/>
         <v>15.116212650000001</v>
       </c>
-      <c r="Y16" s="34">
+      <c r="Y16" s="52">
         <f t="shared" si="7"/>
         <v>15.740651850000003</v>
       </c>
-      <c r="Z16" s="34">
+      <c r="Z16" s="52">
         <f t="shared" si="7"/>
         <v>9.5642431500000029</v>
       </c>
-      <c r="AA16" s="34">
+      <c r="AA16" s="52">
         <f t="shared" si="7"/>
         <v>23.6481168</v>
       </c>
-      <c r="AB16" s="34">
+      <c r="AB16" s="52">
         <f t="shared" si="7"/>
         <v>4.0223452500000008</v>
       </c>
-      <c r="AC16" s="34">
+      <c r="AC16" s="52">
         <f t="shared" si="7"/>
         <v>15.774643500000002</v>
       </c>
-      <c r="AD16" s="34">
+      <c r="AD16" s="52">
         <f t="shared" si="7"/>
         <v>7.4403945000000018</v>
       </c>
-      <c r="AE16" s="34">
+      <c r="AE16" s="52">
         <f t="shared" si="7"/>
         <v>7.0614505500000018</v>
       </c>
-      <c r="AF16" s="34">
+      <c r="AF16" s="52">
         <f t="shared" si="7"/>
         <v>9.2872741500000018</v>
       </c>
-      <c r="AG16" s="34">
+      <c r="AG16" s="52">
         <f t="shared" si="7"/>
         <v>17.117943150000002</v>
       </c>
-      <c r="AH16" s="34">
+      <c r="AH16" s="52">
         <f t="shared" si="7"/>
         <v>8.4047502000000005</v>
       </c>
       <c r="AI16" s="32"/>
     </row>
-    <row r="17" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="32"/>
       <c r="E17" s="30">
         <v>2050</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G17" s="32"/>
-      <c r="H17" s="34">
+      <c r="H17" s="52">
         <f>H16*1.37</f>
         <v>554.98168213950021</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="52">
         <f t="shared" ref="I17:AH17" si="8">I16*1.37</f>
         <v>9.0929426280000012</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="52">
         <f t="shared" si="8"/>
         <v>116.72150975100004</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="52">
         <f t="shared" si="8"/>
         <v>24.881409399000006</v>
       </c>
-      <c r="L17" s="34">
+      <c r="L17" s="52">
         <f t="shared" si="8"/>
         <v>12.520043728500003</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="52">
         <f t="shared" si="8"/>
         <v>9.2481711630000021</v>
       </c>
-      <c r="N17" s="34">
+      <c r="N17" s="52">
         <f t="shared" si="8"/>
         <v>6.0866833334999999</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="52">
         <f t="shared" si="8"/>
         <v>12.338943771000006</v>
       </c>
-      <c r="P17" s="34">
+      <c r="P17" s="52">
         <f t="shared" si="8"/>
         <v>22.216652881500007</v>
       </c>
-      <c r="Q17" s="34">
+      <c r="Q17" s="52">
         <f t="shared" si="8"/>
         <v>10.412385175500003</v>
       </c>
-      <c r="R17" s="34">
+      <c r="R17" s="52">
         <f t="shared" si="8"/>
         <v>13.099563592500006</v>
       </c>
-      <c r="S17" s="34">
+      <c r="S17" s="52">
         <f t="shared" si="8"/>
         <v>21.057613153500004</v>
       </c>
-      <c r="T17" s="34">
+      <c r="T17" s="52">
         <f t="shared" si="8"/>
         <v>15.234818329500007</v>
       </c>
-      <c r="U17" s="34">
+      <c r="U17" s="52">
         <f t="shared" si="8"/>
         <v>15.208946907000005</v>
       </c>
-      <c r="V17" s="34">
+      <c r="V17" s="52">
         <f t="shared" si="8"/>
         <v>65.192535177000025</v>
       </c>
-      <c r="W17" s="34">
+      <c r="W17" s="52">
         <f t="shared" si="8"/>
         <v>19.215567871500003</v>
       </c>
-      <c r="X17" s="34">
+      <c r="X17" s="52">
         <f t="shared" si="8"/>
         <v>20.709211330500004</v>
       </c>
-      <c r="Y17" s="34">
+      <c r="Y17" s="52">
         <f t="shared" si="8"/>
         <v>21.564693034500007</v>
       </c>
-      <c r="Z17" s="34">
+      <c r="Z17" s="52">
         <f t="shared" si="8"/>
         <v>13.103013115500005</v>
       </c>
-      <c r="AA17" s="34">
+      <c r="AA17" s="52">
         <f t="shared" si="8"/>
         <v>32.397920016</v>
       </c>
-      <c r="AB17" s="34">
+      <c r="AB17" s="52">
         <f t="shared" si="8"/>
         <v>5.5106129925000014</v>
       </c>
-      <c r="AC17" s="34">
+      <c r="AC17" s="52">
         <f t="shared" si="8"/>
         <v>21.611261595000006</v>
       </c>
-      <c r="AD17" s="34">
+      <c r="AD17" s="52">
         <f t="shared" si="8"/>
         <v>10.193340465000004</v>
       </c>
-      <c r="AE17" s="34">
+      <c r="AE17" s="52">
         <f t="shared" si="8"/>
         <v>9.6741872535000031</v>
       </c>
-      <c r="AF17" s="34">
+      <c r="AF17" s="52">
         <f t="shared" si="8"/>
         <v>12.723565585500003</v>
       </c>
-      <c r="AG17" s="34">
+      <c r="AG17" s="52">
         <f t="shared" si="8"/>
         <v>23.451582115500006</v>
       </c>
-      <c r="AH17" s="34">
+      <c r="AH17" s="52">
         <f t="shared" si="8"/>
         <v>11.514507774000002</v>
       </c>
@@ -4630,120 +4632,120 @@
     </row>
     <row r="18" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="32"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="30">
         <v>2070</v>
       </c>
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G18" s="32"/>
-      <c r="H18" s="34">
+      <c r="H18" s="52">
         <f>H14*2.5</f>
         <v>844.65412500000002</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="52">
         <f t="shared" ref="I18:AH18" si="9">I14*2.5</f>
         <v>13.838999999999999</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="52">
         <f t="shared" si="9"/>
         <v>177.64425000000003</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="52">
         <f t="shared" si="9"/>
         <v>37.868250000000003</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="52">
         <f t="shared" si="9"/>
         <v>19.054874999999999</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="52">
         <f t="shared" si="9"/>
         <v>14.07525</v>
       </c>
-      <c r="N18" s="34">
+      <c r="N18" s="52">
         <f t="shared" si="9"/>
         <v>9.2636249999999993</v>
       </c>
-      <c r="O18" s="34">
+      <c r="O18" s="52">
         <f t="shared" si="9"/>
         <v>18.779250000000001</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="52">
         <f t="shared" si="9"/>
         <v>33.812624999999997</v>
       </c>
-      <c r="Q18" s="34">
+      <c r="Q18" s="52">
         <f t="shared" si="9"/>
         <v>15.847125</v>
       </c>
-      <c r="R18" s="34">
+      <c r="R18" s="52">
         <f t="shared" si="9"/>
         <v>19.936875000000004</v>
       </c>
-      <c r="S18" s="34">
+      <c r="S18" s="52">
         <f t="shared" si="9"/>
         <v>32.048625000000001</v>
       </c>
-      <c r="T18" s="34">
+      <c r="T18" s="52">
         <f t="shared" si="9"/>
         <v>23.186625000000003</v>
       </c>
-      <c r="U18" s="34">
+      <c r="U18" s="52">
         <f t="shared" si="9"/>
         <v>23.14725</v>
       </c>
-      <c r="V18" s="34">
+      <c r="V18" s="52">
         <f t="shared" si="9"/>
         <v>99.219750000000019</v>
       </c>
-      <c r="W18" s="34">
+      <c r="W18" s="52">
         <f t="shared" si="9"/>
         <v>29.245125000000002</v>
       </c>
-      <c r="X18" s="34">
+      <c r="X18" s="52">
         <f t="shared" si="9"/>
         <v>31.518374999999999</v>
       </c>
-      <c r="Y18" s="34">
+      <c r="Y18" s="52">
         <f t="shared" si="9"/>
         <v>32.820375000000006</v>
       </c>
-      <c r="Z18" s="34">
+      <c r="Z18" s="52">
         <f t="shared" si="9"/>
         <v>19.942125000000001</v>
       </c>
-      <c r="AA18" s="34">
+      <c r="AA18" s="52">
         <f t="shared" si="9"/>
         <v>49.307999999999993</v>
       </c>
-      <c r="AB18" s="34">
+      <c r="AB18" s="52">
         <f t="shared" si="9"/>
         <v>8.3868749999999999</v>
       </c>
-      <c r="AC18" s="34">
+      <c r="AC18" s="52">
         <f t="shared" si="9"/>
         <v>32.891249999999999</v>
       </c>
-      <c r="AD18" s="34">
+      <c r="AD18" s="52">
         <f t="shared" si="9"/>
         <v>15.513750000000002</v>
       </c>
-      <c r="AE18" s="34">
+      <c r="AE18" s="52">
         <f t="shared" si="9"/>
         <v>14.723625</v>
       </c>
-      <c r="AF18" s="34">
+      <c r="AF18" s="52">
         <f t="shared" si="9"/>
         <v>19.364625</v>
       </c>
-      <c r="AG18" s="34">
+      <c r="AG18" s="52">
         <f t="shared" si="9"/>
         <v>35.692124999999997</v>
       </c>
-      <c r="AH18" s="34">
+      <c r="AH18" s="52">
         <f t="shared" si="9"/>
         <v>17.5245</v>
       </c>
@@ -4751,99 +4753,99 @@
     </row>
     <row r="19" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="32"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="32"/>
       <c r="E19" s="33">
         <v>0</v>
       </c>
-      <c r="F19" s="51" t="s">
+      <c r="F19" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G19" s="32"/>
-      <c r="H19" s="53">
+      <c r="H19" s="52">
         <v>5</v>
       </c>
-      <c r="I19" s="53">
+      <c r="I19" s="52">
         <v>5</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="52">
         <v>5</v>
       </c>
-      <c r="K19" s="53">
+      <c r="K19" s="52">
         <v>5</v>
       </c>
-      <c r="L19" s="53">
+      <c r="L19" s="52">
         <v>5</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="52">
         <v>5</v>
       </c>
-      <c r="N19" s="53">
+      <c r="N19" s="52">
         <v>5</v>
       </c>
-      <c r="O19" s="53">
+      <c r="O19" s="52">
         <v>5</v>
       </c>
-      <c r="P19" s="53">
+      <c r="P19" s="52">
         <v>5</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="52">
         <v>5</v>
       </c>
-      <c r="R19" s="53">
+      <c r="R19" s="52">
         <v>5</v>
       </c>
-      <c r="S19" s="53">
+      <c r="S19" s="52">
         <v>5</v>
       </c>
-      <c r="T19" s="53">
+      <c r="T19" s="52">
         <v>5</v>
       </c>
-      <c r="U19" s="53">
+      <c r="U19" s="52">
         <v>5</v>
       </c>
-      <c r="V19" s="53">
+      <c r="V19" s="52">
         <v>5</v>
       </c>
-      <c r="W19" s="53">
+      <c r="W19" s="52">
         <v>5</v>
       </c>
-      <c r="X19" s="53">
+      <c r="X19" s="52">
         <v>5</v>
       </c>
-      <c r="Y19" s="53">
+      <c r="Y19" s="52">
         <v>5</v>
       </c>
-      <c r="Z19" s="53">
+      <c r="Z19" s="52">
         <v>5</v>
       </c>
-      <c r="AA19" s="53">
+      <c r="AA19" s="52">
         <v>5</v>
       </c>
-      <c r="AB19" s="53">
+      <c r="AB19" s="52">
         <v>5</v>
       </c>
-      <c r="AC19" s="53">
+      <c r="AC19" s="52">
         <v>5</v>
       </c>
-      <c r="AD19" s="53">
+      <c r="AD19" s="52">
         <v>5</v>
       </c>
-      <c r="AE19" s="53">
+      <c r="AE19" s="52">
         <v>5</v>
       </c>
-      <c r="AF19" s="53">
+      <c r="AF19" s="52">
         <v>5</v>
       </c>
-      <c r="AG19" s="53">
+      <c r="AG19" s="52">
         <v>5</v>
       </c>
-      <c r="AH19" s="53">
+      <c r="AH19" s="52">
         <v>5</v>
       </c>
       <c r="AI19" s="32"/>
     </row>
-    <row r="20" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
       <c r="C20" s="29" t="s">
         <v>101</v>
@@ -4854,568 +4856,568 @@
       <c r="E20" s="31">
         <v>2018</v>
       </c>
-      <c r="F20" s="55"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="29"/>
-      <c r="H20" s="54">
+      <c r="H20" s="53">
         <v>1</v>
       </c>
-      <c r="I20" s="54">
+      <c r="I20" s="53">
         <v>1</v>
       </c>
-      <c r="J20" s="54">
+      <c r="J20" s="53">
         <v>1</v>
       </c>
-      <c r="K20" s="54">
+      <c r="K20" s="53">
         <v>1</v>
       </c>
-      <c r="L20" s="54">
+      <c r="L20" s="53">
         <v>1</v>
       </c>
-      <c r="M20" s="54">
+      <c r="M20" s="53">
         <v>1</v>
       </c>
-      <c r="N20" s="54">
+      <c r="N20" s="53">
         <v>1</v>
       </c>
-      <c r="O20" s="54">
+      <c r="O20" s="53">
         <v>1</v>
       </c>
-      <c r="P20" s="54">
+      <c r="P20" s="53">
         <v>1</v>
       </c>
-      <c r="Q20" s="54">
+      <c r="Q20" s="53">
         <v>1</v>
       </c>
-      <c r="R20" s="54">
+      <c r="R20" s="53">
         <v>1</v>
       </c>
-      <c r="S20" s="54">
+      <c r="S20" s="53">
         <v>1</v>
       </c>
-      <c r="T20" s="54">
+      <c r="T20" s="53">
         <v>1</v>
       </c>
-      <c r="U20" s="54">
+      <c r="U20" s="53">
         <v>1</v>
       </c>
-      <c r="V20" s="54">
+      <c r="V20" s="53">
         <v>1</v>
       </c>
-      <c r="W20" s="54">
+      <c r="W20" s="53">
         <v>1</v>
       </c>
-      <c r="X20" s="54">
+      <c r="X20" s="53">
         <v>1</v>
       </c>
-      <c r="Y20" s="54">
+      <c r="Y20" s="53">
         <v>1</v>
       </c>
-      <c r="Z20" s="54">
+      <c r="Z20" s="53">
         <v>1</v>
       </c>
-      <c r="AA20" s="54">
+      <c r="AA20" s="53">
         <v>1</v>
       </c>
-      <c r="AB20" s="54">
+      <c r="AB20" s="53">
         <v>1</v>
       </c>
-      <c r="AC20" s="54">
+      <c r="AC20" s="53">
         <v>1</v>
       </c>
-      <c r="AD20" s="54">
+      <c r="AD20" s="53">
         <v>1</v>
       </c>
-      <c r="AE20" s="54">
+      <c r="AE20" s="53">
         <v>1</v>
       </c>
-      <c r="AF20" s="54">
+      <c r="AF20" s="53">
         <v>1</v>
       </c>
-      <c r="AG20" s="54">
+      <c r="AG20" s="53">
         <v>1</v>
       </c>
-      <c r="AH20" s="54">
+      <c r="AH20" s="53">
         <v>1</v>
       </c>
       <c r="AI20" s="32"/>
     </row>
     <row r="21" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+        <v>137</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="30">
         <v>2018</v>
       </c>
-      <c r="F21" s="51" t="s">
+      <c r="F21" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="H21" s="34">
+        <v>139</v>
+      </c>
+      <c r="H21" s="52">
         <f>H44*1.05</f>
         <v>11.58675</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="52">
         <f t="shared" ref="I21:AH21" si="10">I44*1.05</f>
         <v>0.15434999999999999</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="52">
         <f t="shared" si="10"/>
         <v>3.1143000000000005</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="52">
         <f t="shared" si="10"/>
         <v>0.58065000000000011</v>
       </c>
-      <c r="L21" s="34">
+      <c r="L21" s="52">
         <f t="shared" si="10"/>
         <v>0.26145000000000002</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="52">
         <f t="shared" si="10"/>
         <v>0.22785</v>
       </c>
-      <c r="N21" s="34">
+      <c r="N21" s="52">
         <f t="shared" si="10"/>
         <v>0.14070000000000002</v>
       </c>
-      <c r="O21" s="34">
+      <c r="O21" s="52">
         <f t="shared" si="10"/>
         <v>0.3906</v>
       </c>
-      <c r="P21" s="34">
+      <c r="P21" s="52">
         <f t="shared" si="10"/>
         <v>0.50295000000000001</v>
       </c>
-      <c r="Q21" s="34">
+      <c r="Q21" s="52">
         <f t="shared" si="10"/>
         <v>0.17430000000000001</v>
       </c>
-      <c r="R21" s="34">
+      <c r="R21" s="52">
         <f t="shared" si="10"/>
         <v>0.20790000000000003</v>
       </c>
-      <c r="S21" s="34">
+      <c r="S21" s="52">
         <f t="shared" si="10"/>
         <v>0.40845000000000004</v>
       </c>
-      <c r="T21" s="34">
+      <c r="T21" s="52">
         <f t="shared" si="10"/>
         <v>0.21734999999999999</v>
       </c>
-      <c r="U21" s="34">
+      <c r="U21" s="52">
         <f t="shared" si="10"/>
         <v>0.23100000000000001</v>
       </c>
-      <c r="V21" s="34">
+      <c r="V21" s="52">
         <f t="shared" si="10"/>
         <v>1.2253500000000002</v>
       </c>
-      <c r="W21" s="34">
+      <c r="W21" s="52">
         <f t="shared" si="10"/>
         <v>0.27510000000000001</v>
       </c>
-      <c r="X21" s="34">
+      <c r="X21" s="52">
         <f t="shared" si="10"/>
         <v>0.73499999999999999</v>
       </c>
-      <c r="Y21" s="34">
+      <c r="Y21" s="52">
         <f t="shared" si="10"/>
         <v>0.42945</v>
       </c>
-      <c r="Z21" s="34">
+      <c r="Z21" s="52">
         <f t="shared" si="10"/>
         <v>0.21734999999999999</v>
       </c>
-      <c r="AA21" s="34">
+      <c r="AA21" s="52">
         <f t="shared" si="10"/>
         <v>0.57435000000000003</v>
       </c>
-      <c r="AB21" s="34">
+      <c r="AB21" s="52">
         <f t="shared" si="10"/>
         <v>7.7700000000000005E-2</v>
       </c>
-      <c r="AC21" s="34">
+      <c r="AC21" s="52">
         <f t="shared" si="10"/>
         <v>0.27405000000000002</v>
       </c>
-      <c r="AD21" s="34">
+      <c r="AD21" s="52">
         <f t="shared" si="10"/>
         <v>0.15540000000000001</v>
       </c>
-      <c r="AE21" s="34">
+      <c r="AE21" s="52">
         <f t="shared" si="10"/>
         <v>0.21525</v>
       </c>
-      <c r="AF21" s="34">
+      <c r="AF21" s="52">
         <f t="shared" si="10"/>
         <v>0.19320000000000001</v>
       </c>
-      <c r="AG21" s="34">
+      <c r="AG21" s="52">
         <f t="shared" si="10"/>
         <v>0.33390000000000003</v>
       </c>
-      <c r="AH21" s="34">
+      <c r="AH21" s="52">
         <f t="shared" si="10"/>
         <v>0.26880000000000004</v>
       </c>
       <c r="AI21" s="32"/>
     </row>
-    <row r="22" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="32"/>
       <c r="E22" s="30">
         <v>2022</v>
       </c>
-      <c r="F22" s="51" t="s">
+      <c r="F22" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G22" s="32"/>
-      <c r="H22" s="34">
+      <c r="H22" s="52">
         <f>H21</f>
         <v>11.58675</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="52">
         <f t="shared" ref="I22:AH22" si="11">I21</f>
         <v>0.15434999999999999</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="52">
         <f t="shared" si="11"/>
         <v>3.1143000000000005</v>
       </c>
-      <c r="K22" s="34">
+      <c r="K22" s="52">
         <f t="shared" si="11"/>
         <v>0.58065000000000011</v>
       </c>
-      <c r="L22" s="34">
+      <c r="L22" s="52">
         <f t="shared" si="11"/>
         <v>0.26145000000000002</v>
       </c>
-      <c r="M22" s="34">
+      <c r="M22" s="52">
         <f t="shared" si="11"/>
         <v>0.22785</v>
       </c>
-      <c r="N22" s="34">
+      <c r="N22" s="52">
         <f t="shared" si="11"/>
         <v>0.14070000000000002</v>
       </c>
-      <c r="O22" s="34">
+      <c r="O22" s="52">
         <f t="shared" si="11"/>
         <v>0.3906</v>
       </c>
-      <c r="P22" s="34">
+      <c r="P22" s="52">
         <f t="shared" si="11"/>
         <v>0.50295000000000001</v>
       </c>
-      <c r="Q22" s="34">
+      <c r="Q22" s="52">
         <f t="shared" si="11"/>
         <v>0.17430000000000001</v>
       </c>
-      <c r="R22" s="34">
+      <c r="R22" s="52">
         <f t="shared" si="11"/>
         <v>0.20790000000000003</v>
       </c>
-      <c r="S22" s="34">
+      <c r="S22" s="52">
         <f t="shared" si="11"/>
         <v>0.40845000000000004</v>
       </c>
-      <c r="T22" s="34">
+      <c r="T22" s="52">
         <f t="shared" si="11"/>
         <v>0.21734999999999999</v>
       </c>
-      <c r="U22" s="34">
+      <c r="U22" s="52">
         <f t="shared" si="11"/>
         <v>0.23100000000000001</v>
       </c>
-      <c r="V22" s="34">
+      <c r="V22" s="52">
         <f t="shared" si="11"/>
         <v>1.2253500000000002</v>
       </c>
-      <c r="W22" s="34">
+      <c r="W22" s="52">
         <f t="shared" si="11"/>
         <v>0.27510000000000001</v>
       </c>
-      <c r="X22" s="34">
+      <c r="X22" s="52">
         <f t="shared" si="11"/>
         <v>0.73499999999999999</v>
       </c>
-      <c r="Y22" s="34">
+      <c r="Y22" s="52">
         <f t="shared" si="11"/>
         <v>0.42945</v>
       </c>
-      <c r="Z22" s="34">
+      <c r="Z22" s="52">
         <f t="shared" si="11"/>
         <v>0.21734999999999999</v>
       </c>
-      <c r="AA22" s="34">
+      <c r="AA22" s="52">
         <f t="shared" si="11"/>
         <v>0.57435000000000003</v>
       </c>
-      <c r="AB22" s="34">
+      <c r="AB22" s="52">
         <f t="shared" si="11"/>
         <v>7.7700000000000005E-2</v>
       </c>
-      <c r="AC22" s="34">
+      <c r="AC22" s="52">
         <f t="shared" si="11"/>
         <v>0.27405000000000002</v>
       </c>
-      <c r="AD22" s="34">
+      <c r="AD22" s="52">
         <f t="shared" si="11"/>
         <v>0.15540000000000001</v>
       </c>
-      <c r="AE22" s="34">
+      <c r="AE22" s="52">
         <f t="shared" si="11"/>
         <v>0.21525</v>
       </c>
-      <c r="AF22" s="34">
+      <c r="AF22" s="52">
         <f t="shared" si="11"/>
         <v>0.19320000000000001</v>
       </c>
-      <c r="AG22" s="34">
+      <c r="AG22" s="52">
         <f t="shared" si="11"/>
         <v>0.33390000000000003</v>
       </c>
-      <c r="AH22" s="34">
+      <c r="AH22" s="52">
         <f t="shared" si="11"/>
         <v>0.26880000000000004</v>
       </c>
       <c r="AI22" s="32"/>
     </row>
-    <row r="23" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="32"/>
       <c r="E23" s="30">
         <v>2030</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="F23" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G23" s="32"/>
-      <c r="H23" s="34">
+      <c r="H23" s="52">
         <f>H22*1.3</f>
         <v>15.062775</v>
       </c>
-      <c r="I23" s="34">
+      <c r="I23" s="52">
         <f t="shared" ref="I23:AH23" si="12">I22*1.3</f>
         <v>0.200655</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="52">
         <f t="shared" si="12"/>
         <v>4.0485900000000008</v>
       </c>
-      <c r="K23" s="34">
+      <c r="K23" s="52">
         <f t="shared" si="12"/>
         <v>0.75484500000000021</v>
       </c>
-      <c r="L23" s="34">
+      <c r="L23" s="52">
         <f t="shared" si="12"/>
         <v>0.33988500000000005</v>
       </c>
-      <c r="M23" s="34">
+      <c r="M23" s="52">
         <f t="shared" si="12"/>
         <v>0.296205</v>
       </c>
-      <c r="N23" s="34">
+      <c r="N23" s="52">
         <f t="shared" si="12"/>
         <v>0.18291000000000004</v>
       </c>
-      <c r="O23" s="34">
+      <c r="O23" s="52">
         <f t="shared" si="12"/>
         <v>0.50778000000000001</v>
       </c>
-      <c r="P23" s="34">
+      <c r="P23" s="52">
         <f t="shared" si="12"/>
         <v>0.65383500000000006</v>
       </c>
-      <c r="Q23" s="34">
+      <c r="Q23" s="52">
         <f t="shared" si="12"/>
         <v>0.22659000000000001</v>
       </c>
-      <c r="R23" s="34">
+      <c r="R23" s="52">
         <f t="shared" si="12"/>
         <v>0.27027000000000007</v>
       </c>
-      <c r="S23" s="34">
+      <c r="S23" s="52">
         <f t="shared" si="12"/>
         <v>0.53098500000000004</v>
       </c>
-      <c r="T23" s="34">
+      <c r="T23" s="52">
         <f t="shared" si="12"/>
         <v>0.282555</v>
       </c>
-      <c r="U23" s="34">
+      <c r="U23" s="52">
         <f t="shared" si="12"/>
         <v>0.30030000000000001</v>
       </c>
-      <c r="V23" s="34">
+      <c r="V23" s="52">
         <f t="shared" si="12"/>
         <v>1.5929550000000003</v>
       </c>
-      <c r="W23" s="34">
+      <c r="W23" s="52">
         <f t="shared" si="12"/>
         <v>0.35763</v>
       </c>
-      <c r="X23" s="34">
+      <c r="X23" s="52">
         <f t="shared" si="12"/>
         <v>0.95550000000000002</v>
       </c>
-      <c r="Y23" s="34">
+      <c r="Y23" s="52">
         <f t="shared" si="12"/>
         <v>0.55828500000000003</v>
       </c>
-      <c r="Z23" s="34">
+      <c r="Z23" s="52">
         <f t="shared" si="12"/>
         <v>0.282555</v>
       </c>
-      <c r="AA23" s="34">
+      <c r="AA23" s="52">
         <f t="shared" si="12"/>
         <v>0.74665500000000007</v>
       </c>
-      <c r="AB23" s="34">
+      <c r="AB23" s="52">
         <f t="shared" si="12"/>
         <v>0.10101000000000002</v>
       </c>
-      <c r="AC23" s="34">
+      <c r="AC23" s="52">
         <f t="shared" si="12"/>
         <v>0.35626500000000005</v>
       </c>
-      <c r="AD23" s="34">
+      <c r="AD23" s="52">
         <f t="shared" si="12"/>
         <v>0.20202000000000003</v>
       </c>
-      <c r="AE23" s="34">
+      <c r="AE23" s="52">
         <f t="shared" si="12"/>
         <v>0.27982499999999999</v>
       </c>
-      <c r="AF23" s="34">
+      <c r="AF23" s="52">
         <f t="shared" si="12"/>
         <v>0.25116000000000005</v>
       </c>
-      <c r="AG23" s="34">
+      <c r="AG23" s="52">
         <f t="shared" si="12"/>
         <v>0.43407000000000007</v>
       </c>
-      <c r="AH23" s="34">
+      <c r="AH23" s="52">
         <f t="shared" si="12"/>
         <v>0.34944000000000008</v>
       </c>
       <c r="AI23" s="32"/>
     </row>
-    <row r="24" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="32"/>
       <c r="E24" s="30">
         <v>2050</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G24" s="32"/>
-      <c r="H24" s="34">
+      <c r="H24" s="52">
         <f>H23*2.3</f>
         <v>34.644382499999999</v>
       </c>
-      <c r="I24" s="34">
+      <c r="I24" s="52">
         <f t="shared" ref="I24:AH24" si="13">I23*2.3</f>
         <v>0.46150649999999999</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="52">
         <f t="shared" si="13"/>
         <v>9.3117570000000018</v>
       </c>
-      <c r="K24" s="34">
+      <c r="K24" s="52">
         <f t="shared" si="13"/>
         <v>1.7361435000000003</v>
       </c>
-      <c r="L24" s="34">
+      <c r="L24" s="52">
         <f t="shared" si="13"/>
         <v>0.78173550000000003</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="52">
         <f t="shared" si="13"/>
         <v>0.68127149999999992</v>
       </c>
-      <c r="N24" s="34">
+      <c r="N24" s="52">
         <f t="shared" si="13"/>
         <v>0.42069300000000009</v>
       </c>
-      <c r="O24" s="34">
+      <c r="O24" s="52">
         <f t="shared" si="13"/>
         <v>1.167894</v>
       </c>
-      <c r="P24" s="34">
+      <c r="P24" s="52">
         <f t="shared" si="13"/>
         <v>1.5038205</v>
       </c>
-      <c r="Q24" s="34">
+      <c r="Q24" s="52">
         <f t="shared" si="13"/>
         <v>0.52115699999999998</v>
       </c>
-      <c r="R24" s="34">
+      <c r="R24" s="52">
         <f t="shared" si="13"/>
         <v>0.62162100000000009</v>
       </c>
-      <c r="S24" s="34">
+      <c r="S24" s="52">
         <f t="shared" si="13"/>
         <v>1.2212654999999999</v>
       </c>
-      <c r="T24" s="34">
+      <c r="T24" s="52">
         <f t="shared" si="13"/>
         <v>0.64987649999999997</v>
       </c>
-      <c r="U24" s="34">
+      <c r="U24" s="52">
         <f t="shared" si="13"/>
         <v>0.69069000000000003</v>
       </c>
-      <c r="V24" s="34">
+      <c r="V24" s="52">
         <f t="shared" si="13"/>
         <v>3.6637965000000006</v>
       </c>
-      <c r="W24" s="34">
+      <c r="W24" s="52">
         <f t="shared" si="13"/>
         <v>0.82254899999999997</v>
       </c>
-      <c r="X24" s="34">
+      <c r="X24" s="52">
         <f t="shared" si="13"/>
         <v>2.1976499999999999</v>
       </c>
-      <c r="Y24" s="34">
+      <c r="Y24" s="52">
         <f t="shared" si="13"/>
         <v>1.2840555</v>
       </c>
-      <c r="Z24" s="34">
+      <c r="Z24" s="52">
         <f t="shared" si="13"/>
         <v>0.64987649999999997</v>
       </c>
-      <c r="AA24" s="34">
+      <c r="AA24" s="52">
         <f t="shared" si="13"/>
         <v>1.7173065000000001</v>
       </c>
-      <c r="AB24" s="34">
+      <c r="AB24" s="52">
         <f t="shared" si="13"/>
         <v>0.23232300000000003</v>
       </c>
-      <c r="AC24" s="34">
+      <c r="AC24" s="52">
         <f t="shared" si="13"/>
         <v>0.81940950000000001</v>
       </c>
-      <c r="AD24" s="34">
+      <c r="AD24" s="52">
         <f t="shared" si="13"/>
         <v>0.46464600000000006</v>
       </c>
-      <c r="AE24" s="34">
+      <c r="AE24" s="52">
         <f t="shared" si="13"/>
         <v>0.64359749999999993</v>
       </c>
-      <c r="AF24" s="34">
+      <c r="AF24" s="52">
         <f t="shared" si="13"/>
         <v>0.57766800000000007</v>
       </c>
-      <c r="AG24" s="34">
+      <c r="AG24" s="52">
         <f t="shared" si="13"/>
         <v>0.99836100000000005</v>
       </c>
-      <c r="AH24" s="34">
+      <c r="AH24" s="52">
         <f t="shared" si="13"/>
         <v>0.80371200000000009</v>
       </c>
@@ -5423,120 +5425,120 @@
     </row>
     <row r="25" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="32"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="30">
         <v>2070</v>
       </c>
-      <c r="F25" s="51" t="s">
+      <c r="F25" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G25" s="32"/>
-      <c r="H25" s="34">
+      <c r="H25" s="52">
         <f>H21*3.4</f>
         <v>39.394950000000001</v>
       </c>
-      <c r="I25" s="34">
+      <c r="I25" s="52">
         <f t="shared" ref="I25:AH25" si="14">I21*3.4</f>
         <v>0.52478999999999998</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="52">
         <f t="shared" si="14"/>
         <v>10.588620000000001</v>
       </c>
-      <c r="K25" s="34">
+      <c r="K25" s="52">
         <f t="shared" si="14"/>
         <v>1.9742100000000002</v>
       </c>
-      <c r="L25" s="34">
+      <c r="L25" s="52">
         <f t="shared" si="14"/>
         <v>0.88893</v>
       </c>
-      <c r="M25" s="34">
+      <c r="M25" s="52">
         <f t="shared" si="14"/>
         <v>0.77468999999999999</v>
       </c>
-      <c r="N25" s="34">
+      <c r="N25" s="52">
         <f t="shared" si="14"/>
         <v>0.47838000000000003</v>
       </c>
-      <c r="O25" s="34">
+      <c r="O25" s="52">
         <f t="shared" si="14"/>
         <v>1.3280399999999999</v>
       </c>
-      <c r="P25" s="34">
+      <c r="P25" s="52">
         <f t="shared" si="14"/>
         <v>1.7100299999999999</v>
       </c>
-      <c r="Q25" s="34">
+      <c r="Q25" s="52">
         <f t="shared" si="14"/>
         <v>0.59262000000000004</v>
       </c>
-      <c r="R25" s="34">
+      <c r="R25" s="52">
         <f t="shared" si="14"/>
         <v>0.70686000000000004</v>
       </c>
-      <c r="S25" s="34">
+      <c r="S25" s="52">
         <f t="shared" si="14"/>
         <v>1.38873</v>
       </c>
-      <c r="T25" s="34">
+      <c r="T25" s="52">
         <f t="shared" si="14"/>
         <v>0.73898999999999992</v>
       </c>
-      <c r="U25" s="34">
+      <c r="U25" s="52">
         <f t="shared" si="14"/>
         <v>0.78539999999999999</v>
       </c>
-      <c r="V25" s="34">
+      <c r="V25" s="52">
         <f t="shared" si="14"/>
         <v>4.1661900000000003</v>
       </c>
-      <c r="W25" s="34">
+      <c r="W25" s="52">
         <f t="shared" si="14"/>
         <v>0.93534000000000006</v>
       </c>
-      <c r="X25" s="34">
+      <c r="X25" s="52">
         <f t="shared" si="14"/>
         <v>2.4990000000000001</v>
       </c>
-      <c r="Y25" s="34">
+      <c r="Y25" s="52">
         <f t="shared" si="14"/>
         <v>1.4601299999999999</v>
       </c>
-      <c r="Z25" s="34">
+      <c r="Z25" s="52">
         <f t="shared" si="14"/>
         <v>0.73898999999999992</v>
       </c>
-      <c r="AA25" s="34">
+      <c r="AA25" s="52">
         <f t="shared" si="14"/>
         <v>1.95279</v>
       </c>
-      <c r="AB25" s="34">
+      <c r="AB25" s="52">
         <f t="shared" si="14"/>
         <v>0.26418000000000003</v>
       </c>
-      <c r="AC25" s="34">
+      <c r="AC25" s="52">
         <f t="shared" si="14"/>
         <v>0.93176999999999999</v>
       </c>
-      <c r="AD25" s="34">
+      <c r="AD25" s="52">
         <f t="shared" si="14"/>
         <v>0.52836000000000005</v>
       </c>
-      <c r="AE25" s="34">
+      <c r="AE25" s="52">
         <f t="shared" si="14"/>
         <v>0.73185</v>
       </c>
-      <c r="AF25" s="34">
+      <c r="AF25" s="52">
         <f t="shared" si="14"/>
         <v>0.65688000000000002</v>
       </c>
-      <c r="AG25" s="34">
+      <c r="AG25" s="52">
         <f t="shared" si="14"/>
         <v>1.1352600000000002</v>
       </c>
-      <c r="AH25" s="34">
+      <c r="AH25" s="52">
         <f t="shared" si="14"/>
         <v>0.91392000000000007</v>
       </c>
@@ -5544,102 +5546,102 @@
     </row>
     <row r="26" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="32"/>
-      <c r="C26" s="51"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="32"/>
       <c r="E26" s="33">
         <v>0</v>
       </c>
-      <c r="F26" s="51" t="s">
+      <c r="F26" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G26" s="32"/>
-      <c r="H26" s="53">
+      <c r="H26" s="52">
         <v>5</v>
       </c>
-      <c r="I26" s="53">
+      <c r="I26" s="52">
         <v>5</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="52">
         <v>5</v>
       </c>
-      <c r="K26" s="53">
+      <c r="K26" s="52">
         <v>5</v>
       </c>
-      <c r="L26" s="53">
+      <c r="L26" s="52">
         <v>5</v>
       </c>
-      <c r="M26" s="53">
+      <c r="M26" s="52">
         <v>5</v>
       </c>
-      <c r="N26" s="53">
+      <c r="N26" s="52">
         <v>5</v>
       </c>
-      <c r="O26" s="53">
+      <c r="O26" s="52">
         <v>5</v>
       </c>
-      <c r="P26" s="53">
+      <c r="P26" s="52">
         <v>5</v>
       </c>
-      <c r="Q26" s="53">
+      <c r="Q26" s="52">
         <v>5</v>
       </c>
-      <c r="R26" s="53">
+      <c r="R26" s="52">
         <v>5</v>
       </c>
-      <c r="S26" s="53">
+      <c r="S26" s="52">
         <v>5</v>
       </c>
-      <c r="T26" s="53">
+      <c r="T26" s="52">
         <v>5</v>
       </c>
-      <c r="U26" s="53">
+      <c r="U26" s="52">
         <v>5</v>
       </c>
-      <c r="V26" s="53">
+      <c r="V26" s="52">
         <v>5</v>
       </c>
-      <c r="W26" s="53">
+      <c r="W26" s="52">
         <v>5</v>
       </c>
-      <c r="X26" s="53">
+      <c r="X26" s="52">
         <v>5</v>
       </c>
-      <c r="Y26" s="53">
+      <c r="Y26" s="52">
         <v>5</v>
       </c>
-      <c r="Z26" s="53">
+      <c r="Z26" s="52">
         <v>5</v>
       </c>
-      <c r="AA26" s="53">
+      <c r="AA26" s="52">
         <v>5</v>
       </c>
-      <c r="AB26" s="53">
+      <c r="AB26" s="52">
         <v>5</v>
       </c>
-      <c r="AC26" s="53">
+      <c r="AC26" s="52">
         <v>5</v>
       </c>
-      <c r="AD26" s="53">
+      <c r="AD26" s="52">
         <v>5</v>
       </c>
-      <c r="AE26" s="53">
+      <c r="AE26" s="52">
         <v>5</v>
       </c>
-      <c r="AF26" s="53">
+      <c r="AF26" s="52">
         <v>5</v>
       </c>
-      <c r="AG26" s="53">
+      <c r="AG26" s="52">
         <v>5</v>
       </c>
-      <c r="AH26" s="53">
+      <c r="AH26" s="52">
         <v>5</v>
       </c>
       <c r="AI26" s="32"/>
     </row>
-    <row r="27" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="29"/>
       <c r="C27" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>9</v>
@@ -5647,687 +5649,687 @@
       <c r="E27" s="31">
         <v>2018</v>
       </c>
-      <c r="F27" s="55"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="29"/>
-      <c r="H27" s="54">
+      <c r="H27" s="53">
         <v>1</v>
       </c>
-      <c r="I27" s="54">
+      <c r="I27" s="53">
         <v>1</v>
       </c>
-      <c r="J27" s="54">
+      <c r="J27" s="53">
         <v>1</v>
       </c>
-      <c r="K27" s="54">
+      <c r="K27" s="53">
         <v>1</v>
       </c>
-      <c r="L27" s="54">
+      <c r="L27" s="53">
         <v>1</v>
       </c>
-      <c r="M27" s="54">
+      <c r="M27" s="53">
         <v>1</v>
       </c>
-      <c r="N27" s="54">
+      <c r="N27" s="53">
         <v>1</v>
       </c>
-      <c r="O27" s="54">
+      <c r="O27" s="53">
         <v>1</v>
       </c>
-      <c r="P27" s="54">
+      <c r="P27" s="53">
         <v>1</v>
       </c>
-      <c r="Q27" s="54">
+      <c r="Q27" s="53">
         <v>1</v>
       </c>
-      <c r="R27" s="54">
+      <c r="R27" s="53">
         <v>1</v>
       </c>
-      <c r="S27" s="54">
+      <c r="S27" s="53">
         <v>1</v>
       </c>
-      <c r="T27" s="54">
+      <c r="T27" s="53">
         <v>1</v>
       </c>
-      <c r="U27" s="54">
+      <c r="U27" s="53">
         <v>1</v>
       </c>
-      <c r="V27" s="54">
+      <c r="V27" s="53">
         <v>1</v>
       </c>
-      <c r="W27" s="54">
+      <c r="W27" s="53">
         <v>1</v>
       </c>
-      <c r="X27" s="54">
+      <c r="X27" s="53">
         <v>1</v>
       </c>
-      <c r="Y27" s="54">
+      <c r="Y27" s="53">
         <v>1</v>
       </c>
-      <c r="Z27" s="54">
+      <c r="Z27" s="53">
         <v>1</v>
       </c>
-      <c r="AA27" s="54">
+      <c r="AA27" s="53">
         <v>1</v>
       </c>
-      <c r="AB27" s="54">
+      <c r="AB27" s="53">
         <v>1</v>
       </c>
-      <c r="AC27" s="54">
+      <c r="AC27" s="53">
         <v>1</v>
       </c>
-      <c r="AD27" s="54">
+      <c r="AD27" s="53">
         <v>1</v>
       </c>
-      <c r="AE27" s="54">
+      <c r="AE27" s="53">
         <v>1</v>
       </c>
-      <c r="AF27" s="54">
+      <c r="AF27" s="53">
         <v>1</v>
       </c>
-      <c r="AG27" s="54">
+      <c r="AG27" s="53">
         <v>1</v>
       </c>
-      <c r="AH27" s="54">
+      <c r="AH27" s="53">
         <v>1</v>
       </c>
       <c r="AI27" s="32"/>
     </row>
     <row r="28" spans="2:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
+        <v>140</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="30">
         <v>2018</v>
       </c>
-      <c r="F28" s="51" t="s">
+      <c r="F28" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="H28" s="34">
+        <v>142</v>
+      </c>
+      <c r="H28" s="57">
         <f>H45*1.1</f>
         <v>23.812800000000006</v>
       </c>
-      <c r="I28" s="34">
-        <f t="shared" ref="I28:AH28" si="15">I45*1.1</f>
+      <c r="I28" s="52">
+        <f>I45*1.1</f>
         <v>0.42900000000000005</v>
       </c>
-      <c r="J28" s="34">
-        <f t="shared" si="15"/>
+      <c r="J28" s="52">
+        <f t="shared" ref="I28:AH28" si="15">J45*1.1</f>
         <v>4.2713000000000001</v>
       </c>
-      <c r="K28" s="34">
+      <c r="K28" s="52">
         <f t="shared" si="15"/>
         <v>1.2232000000000003</v>
       </c>
-      <c r="L28" s="34">
+      <c r="L28" s="52">
         <f t="shared" si="15"/>
         <v>0.7843</v>
       </c>
-      <c r="M28" s="34">
+      <c r="M28" s="52">
         <f t="shared" si="15"/>
         <v>0.50050000000000006</v>
       </c>
-      <c r="N28" s="34">
+      <c r="N28" s="52">
         <f t="shared" si="15"/>
         <v>0.30360000000000004</v>
       </c>
-      <c r="O28" s="34">
+      <c r="O28" s="52">
         <f t="shared" si="15"/>
         <v>0.67870000000000008</v>
       </c>
-      <c r="P28" s="34">
+      <c r="P28" s="52">
         <f t="shared" si="15"/>
         <v>1.5664</v>
       </c>
-      <c r="Q28" s="34">
+      <c r="Q28" s="52">
         <f t="shared" si="15"/>
         <v>0.35530000000000006</v>
       </c>
-      <c r="R28" s="34">
+      <c r="R28" s="52">
         <f t="shared" si="15"/>
         <v>0.34760000000000002</v>
       </c>
-      <c r="S28" s="34">
+      <c r="S28" s="52">
         <f t="shared" si="15"/>
         <v>1.5289999999999999</v>
       </c>
-      <c r="T28" s="34">
+      <c r="T28" s="52">
         <f t="shared" si="15"/>
         <v>0.43560000000000004</v>
       </c>
-      <c r="U28" s="34">
+      <c r="U28" s="52">
         <f t="shared" si="15"/>
         <v>0.43670000000000003</v>
       </c>
-      <c r="V28" s="34">
+      <c r="V28" s="52">
         <f t="shared" si="15"/>
         <v>2.8138000000000001</v>
       </c>
-      <c r="W28" s="34">
+      <c r="W28" s="52">
         <f t="shared" si="15"/>
         <v>0.5676000000000001</v>
       </c>
-      <c r="X28" s="34">
+      <c r="X28" s="52">
         <f t="shared" si="15"/>
         <v>1.0351000000000001</v>
       </c>
-      <c r="Y28" s="34">
+      <c r="Y28" s="52">
         <f t="shared" si="15"/>
         <v>1.1550000000000002</v>
       </c>
-      <c r="Z28" s="34">
+      <c r="Z28" s="52">
         <f t="shared" si="15"/>
         <v>0.39380000000000004</v>
       </c>
-      <c r="AA28" s="34">
+      <c r="AA28" s="52">
         <f t="shared" si="15"/>
         <v>1.1286</v>
       </c>
-      <c r="AB28" s="34">
+      <c r="AB28" s="52">
         <f t="shared" si="15"/>
         <v>0.14850000000000002</v>
       </c>
-      <c r="AC28" s="34">
+      <c r="AC28" s="52">
         <f t="shared" si="15"/>
         <v>0.627</v>
       </c>
-      <c r="AD28" s="34">
+      <c r="AD28" s="52">
         <f t="shared" si="15"/>
         <v>0.35860000000000003</v>
       </c>
-      <c r="AE28" s="34">
+      <c r="AE28" s="52">
         <f t="shared" si="15"/>
         <v>0.25520000000000004</v>
       </c>
-      <c r="AF28" s="34">
+      <c r="AF28" s="52">
         <f t="shared" si="15"/>
         <v>0.53680000000000005</v>
       </c>
-      <c r="AG28" s="34">
+      <c r="AG28" s="52">
         <f t="shared" si="15"/>
         <v>0.79200000000000004</v>
       </c>
-      <c r="AH28" s="34">
+      <c r="AH28" s="52">
         <f t="shared" si="15"/>
         <v>1.1396000000000002</v>
       </c>
       <c r="AI28" s="32"/>
     </row>
-    <row r="29" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="32"/>
       <c r="E29" s="30">
         <v>2022</v>
       </c>
-      <c r="F29" s="51" t="s">
+      <c r="F29" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G29" s="32"/>
-      <c r="H29" s="34">
-        <f>H28</f>
-        <v>23.812800000000006</v>
-      </c>
-      <c r="I29" s="34">
+      <c r="H29" s="57">
+        <f>H28*1.05</f>
+        <v>25.003440000000008</v>
+      </c>
+      <c r="I29" s="52">
         <f t="shared" ref="I29:AH29" si="16">I28</f>
         <v>0.42900000000000005</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="52">
         <f t="shared" si="16"/>
         <v>4.2713000000000001</v>
       </c>
-      <c r="K29" s="34">
+      <c r="K29" s="52">
         <f t="shared" si="16"/>
         <v>1.2232000000000003</v>
       </c>
-      <c r="L29" s="34">
+      <c r="L29" s="52">
         <f t="shared" si="16"/>
         <v>0.7843</v>
       </c>
-      <c r="M29" s="34">
+      <c r="M29" s="52">
         <f t="shared" si="16"/>
         <v>0.50050000000000006</v>
       </c>
-      <c r="N29" s="34">
+      <c r="N29" s="52">
         <f t="shared" si="16"/>
         <v>0.30360000000000004</v>
       </c>
-      <c r="O29" s="34">
+      <c r="O29" s="52">
         <f t="shared" si="16"/>
         <v>0.67870000000000008</v>
       </c>
-      <c r="P29" s="34">
+      <c r="P29" s="52">
         <f t="shared" si="16"/>
         <v>1.5664</v>
       </c>
-      <c r="Q29" s="34">
+      <c r="Q29" s="52">
         <f t="shared" si="16"/>
         <v>0.35530000000000006</v>
       </c>
-      <c r="R29" s="34">
+      <c r="R29" s="52">
         <f t="shared" si="16"/>
         <v>0.34760000000000002</v>
       </c>
-      <c r="S29" s="34">
+      <c r="S29" s="52">
         <f t="shared" si="16"/>
         <v>1.5289999999999999</v>
       </c>
-      <c r="T29" s="34">
+      <c r="T29" s="52">
         <f t="shared" si="16"/>
         <v>0.43560000000000004</v>
       </c>
-      <c r="U29" s="34">
+      <c r="U29" s="52">
         <f t="shared" si="16"/>
         <v>0.43670000000000003</v>
       </c>
-      <c r="V29" s="34">
+      <c r="V29" s="52">
         <f t="shared" si="16"/>
         <v>2.8138000000000001</v>
       </c>
-      <c r="W29" s="34">
+      <c r="W29" s="52">
         <f t="shared" si="16"/>
         <v>0.5676000000000001</v>
       </c>
-      <c r="X29" s="34">
+      <c r="X29" s="52">
         <f t="shared" si="16"/>
         <v>1.0351000000000001</v>
       </c>
-      <c r="Y29" s="34">
+      <c r="Y29" s="52">
         <f t="shared" si="16"/>
         <v>1.1550000000000002</v>
       </c>
-      <c r="Z29" s="34">
+      <c r="Z29" s="52">
         <f t="shared" si="16"/>
         <v>0.39380000000000004</v>
       </c>
-      <c r="AA29" s="34">
+      <c r="AA29" s="52">
         <f t="shared" si="16"/>
         <v>1.1286</v>
       </c>
-      <c r="AB29" s="34">
+      <c r="AB29" s="52">
         <f t="shared" si="16"/>
         <v>0.14850000000000002</v>
       </c>
-      <c r="AC29" s="34">
+      <c r="AC29" s="52">
         <f t="shared" si="16"/>
         <v>0.627</v>
       </c>
-      <c r="AD29" s="34">
+      <c r="AD29" s="52">
         <f t="shared" si="16"/>
         <v>0.35860000000000003</v>
       </c>
-      <c r="AE29" s="34">
+      <c r="AE29" s="52">
         <f t="shared" si="16"/>
         <v>0.25520000000000004</v>
       </c>
-      <c r="AF29" s="34">
+      <c r="AF29" s="52">
         <f t="shared" si="16"/>
         <v>0.53680000000000005</v>
       </c>
-      <c r="AG29" s="34">
+      <c r="AG29" s="52">
         <f t="shared" si="16"/>
         <v>0.79200000000000004</v>
       </c>
-      <c r="AH29" s="34">
+      <c r="AH29" s="52">
         <f t="shared" si="16"/>
         <v>1.1396000000000002</v>
       </c>
       <c r="AI29" s="32"/>
     </row>
-    <row r="30" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="32"/>
       <c r="E30" s="30">
         <v>2030</v>
       </c>
-      <c r="F30" s="51" t="s">
+      <c r="F30" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G30" s="32"/>
-      <c r="H30" s="34">
-        <f>H29*1.3</f>
-        <v>30.956640000000011</v>
-      </c>
-      <c r="I30" s="34">
+      <c r="H30" s="57">
+        <f>H29*1.25</f>
+        <v>31.254300000000011</v>
+      </c>
+      <c r="I30" s="52">
         <f t="shared" ref="I30:AH30" si="17">I29*1.3</f>
         <v>0.55770000000000008</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="52">
         <f t="shared" si="17"/>
         <v>5.5526900000000001</v>
       </c>
-      <c r="K30" s="34">
+      <c r="K30" s="52">
         <f t="shared" si="17"/>
         <v>1.5901600000000005</v>
       </c>
-      <c r="L30" s="34">
+      <c r="L30" s="52">
         <f t="shared" si="17"/>
         <v>1.01959</v>
       </c>
-      <c r="M30" s="34">
+      <c r="M30" s="52">
         <f t="shared" si="17"/>
         <v>0.65065000000000006</v>
       </c>
-      <c r="N30" s="34">
+      <c r="N30" s="52">
         <f t="shared" si="17"/>
         <v>0.39468000000000009</v>
       </c>
-      <c r="O30" s="34">
+      <c r="O30" s="52">
         <f t="shared" si="17"/>
         <v>0.88231000000000015</v>
       </c>
-      <c r="P30" s="34">
+      <c r="P30" s="52">
         <f t="shared" si="17"/>
         <v>2.0363199999999999</v>
       </c>
-      <c r="Q30" s="34">
+      <c r="Q30" s="52">
         <f t="shared" si="17"/>
         <v>0.46189000000000008</v>
       </c>
-      <c r="R30" s="34">
+      <c r="R30" s="52">
         <f t="shared" si="17"/>
         <v>0.45188000000000006</v>
       </c>
-      <c r="S30" s="34">
+      <c r="S30" s="52">
         <f t="shared" si="17"/>
         <v>1.9877</v>
       </c>
-      <c r="T30" s="34">
+      <c r="T30" s="52">
         <f t="shared" si="17"/>
         <v>0.56628000000000012</v>
       </c>
-      <c r="U30" s="34">
+      <c r="U30" s="52">
         <f t="shared" si="17"/>
         <v>0.56771000000000005</v>
       </c>
-      <c r="V30" s="34">
+      <c r="V30" s="52">
         <f t="shared" si="17"/>
         <v>3.6579400000000004</v>
       </c>
-      <c r="W30" s="34">
+      <c r="W30" s="52">
         <f t="shared" si="17"/>
         <v>0.7378800000000002</v>
       </c>
-      <c r="X30" s="34">
+      <c r="X30" s="52">
         <f t="shared" si="17"/>
         <v>1.3456300000000003</v>
       </c>
-      <c r="Y30" s="34">
+      <c r="Y30" s="52">
         <f t="shared" si="17"/>
         <v>1.5015000000000003</v>
       </c>
-      <c r="Z30" s="34">
+      <c r="Z30" s="52">
         <f t="shared" si="17"/>
         <v>0.51194000000000006</v>
       </c>
-      <c r="AA30" s="34">
+      <c r="AA30" s="52">
         <f t="shared" si="17"/>
         <v>1.4671800000000002</v>
       </c>
-      <c r="AB30" s="34">
+      <c r="AB30" s="52">
         <f t="shared" si="17"/>
         <v>0.19305000000000003</v>
       </c>
-      <c r="AC30" s="34">
+      <c r="AC30" s="52">
         <f t="shared" si="17"/>
         <v>0.81510000000000005</v>
       </c>
-      <c r="AD30" s="34">
+      <c r="AD30" s="52">
         <f t="shared" si="17"/>
         <v>0.46618000000000004</v>
       </c>
-      <c r="AE30" s="34">
+      <c r="AE30" s="52">
         <f t="shared" si="17"/>
         <v>0.33176000000000005</v>
       </c>
-      <c r="AF30" s="34">
+      <c r="AF30" s="52">
         <f t="shared" si="17"/>
         <v>0.69784000000000013</v>
       </c>
-      <c r="AG30" s="34">
+      <c r="AG30" s="52">
         <f t="shared" si="17"/>
         <v>1.0296000000000001</v>
       </c>
-      <c r="AH30" s="34">
+      <c r="AH30" s="52">
         <f t="shared" si="17"/>
         <v>1.4814800000000004</v>
       </c>
       <c r="AI30" s="32"/>
     </row>
-    <row r="31" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="32"/>
       <c r="E31" s="30">
         <v>2050</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G31" s="32"/>
-      <c r="H31" s="34">
+      <c r="H31" s="57">
         <f>H30*1.9</f>
-        <v>58.817616000000015</v>
-      </c>
-      <c r="I31" s="34">
+        <v>59.383170000000021</v>
+      </c>
+      <c r="I31" s="52">
         <f t="shared" ref="I31:AH31" si="18">I30*1.9</f>
         <v>1.0596300000000001</v>
       </c>
-      <c r="J31" s="34">
+      <c r="J31" s="52">
         <f t="shared" si="18"/>
         <v>10.550110999999999</v>
       </c>
-      <c r="K31" s="34">
+      <c r="K31" s="52">
         <f t="shared" si="18"/>
         <v>3.0213040000000007</v>
       </c>
-      <c r="L31" s="34">
+      <c r="L31" s="52">
         <f t="shared" si="18"/>
         <v>1.9372209999999999</v>
       </c>
-      <c r="M31" s="34">
+      <c r="M31" s="52">
         <f t="shared" si="18"/>
         <v>1.236235</v>
       </c>
-      <c r="N31" s="34">
+      <c r="N31" s="52">
         <f t="shared" si="18"/>
         <v>0.74989200000000011</v>
       </c>
-      <c r="O31" s="34">
+      <c r="O31" s="52">
         <f t="shared" si="18"/>
         <v>1.6763890000000001</v>
       </c>
-      <c r="P31" s="34">
+      <c r="P31" s="52">
         <f t="shared" si="18"/>
         <v>3.8690079999999996</v>
       </c>
-      <c r="Q31" s="34">
+      <c r="Q31" s="52">
         <f t="shared" si="18"/>
         <v>0.87759100000000012</v>
       </c>
-      <c r="R31" s="34">
+      <c r="R31" s="52">
         <f t="shared" si="18"/>
         <v>0.85857200000000011</v>
       </c>
-      <c r="S31" s="34">
+      <c r="S31" s="52">
         <f t="shared" si="18"/>
         <v>3.7766299999999999</v>
       </c>
-      <c r="T31" s="34">
+      <c r="T31" s="52">
         <f t="shared" si="18"/>
         <v>1.0759320000000001</v>
       </c>
-      <c r="U31" s="34">
+      <c r="U31" s="52">
         <f t="shared" si="18"/>
         <v>1.078649</v>
       </c>
-      <c r="V31" s="34">
+      <c r="V31" s="52">
         <f t="shared" si="18"/>
         <v>6.9500860000000007</v>
       </c>
-      <c r="W31" s="34">
+      <c r="W31" s="52">
         <f t="shared" si="18"/>
         <v>1.4019720000000002</v>
       </c>
-      <c r="X31" s="34">
+      <c r="X31" s="52">
         <f t="shared" si="18"/>
         <v>2.5566970000000007</v>
       </c>
-      <c r="Y31" s="34">
+      <c r="Y31" s="52">
         <f t="shared" si="18"/>
         <v>2.8528500000000006</v>
       </c>
-      <c r="Z31" s="34">
+      <c r="Z31" s="52">
         <f t="shared" si="18"/>
         <v>0.97268600000000005</v>
       </c>
-      <c r="AA31" s="34">
+      <c r="AA31" s="52">
         <f t="shared" si="18"/>
         <v>2.787642</v>
       </c>
-      <c r="AB31" s="34">
+      <c r="AB31" s="52">
         <f t="shared" si="18"/>
         <v>0.36679500000000004</v>
       </c>
-      <c r="AC31" s="34">
+      <c r="AC31" s="52">
         <f t="shared" si="18"/>
         <v>1.5486900000000001</v>
       </c>
-      <c r="AD31" s="34">
+      <c r="AD31" s="52">
         <f t="shared" si="18"/>
         <v>0.88574200000000003</v>
       </c>
-      <c r="AE31" s="34">
+      <c r="AE31" s="52">
         <f t="shared" si="18"/>
         <v>0.63034400000000013</v>
       </c>
-      <c r="AF31" s="34">
+      <c r="AF31" s="52">
         <f t="shared" si="18"/>
         <v>1.3258960000000002</v>
       </c>
-      <c r="AG31" s="34">
+      <c r="AG31" s="52">
         <f t="shared" si="18"/>
         <v>1.95624</v>
       </c>
-      <c r="AH31" s="34">
+      <c r="AH31" s="52">
         <f t="shared" si="18"/>
         <v>2.8148120000000008</v>
       </c>
       <c r="AI31" s="32"/>
     </row>
-    <row r="32" spans="2:35" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:35" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="32"/>
       <c r="E32" s="30">
         <v>2070</v>
       </c>
-      <c r="F32" s="51" t="s">
+      <c r="F32" s="50" t="s">
         <v>96</v>
       </c>
       <c r="G32" s="32"/>
-      <c r="H32" s="34">
+      <c r="H32" s="52">
         <f>H28*3.27</f>
         <v>77.867856000000018</v>
       </c>
-      <c r="I32" s="34">
+      <c r="I32" s="52">
         <f t="shared" ref="I32:AH32" si="19">I28*3.27</f>
         <v>1.4028300000000002</v>
       </c>
-      <c r="J32" s="34">
+      <c r="J32" s="52">
         <f t="shared" si="19"/>
         <v>13.967151000000001</v>
       </c>
-      <c r="K32" s="34">
+      <c r="K32" s="52">
         <f t="shared" si="19"/>
         <v>3.999864000000001</v>
       </c>
-      <c r="L32" s="34">
+      <c r="L32" s="52">
         <f t="shared" si="19"/>
         <v>2.5646610000000001</v>
       </c>
-      <c r="M32" s="34">
+      <c r="M32" s="52">
         <f t="shared" si="19"/>
         <v>1.6366350000000003</v>
       </c>
-      <c r="N32" s="34">
+      <c r="N32" s="52">
         <f t="shared" si="19"/>
         <v>0.9927720000000001</v>
       </c>
-      <c r="O32" s="34">
+      <c r="O32" s="52">
         <f t="shared" si="19"/>
         <v>2.2193490000000002</v>
       </c>
-      <c r="P32" s="34">
+      <c r="P32" s="52">
         <f t="shared" si="19"/>
         <v>5.122128</v>
       </c>
-      <c r="Q32" s="34">
+      <c r="Q32" s="52">
         <f t="shared" si="19"/>
         <v>1.1618310000000003</v>
       </c>
-      <c r="R32" s="34">
+      <c r="R32" s="52">
         <f t="shared" si="19"/>
         <v>1.136652</v>
       </c>
-      <c r="S32" s="34">
+      <c r="S32" s="52">
         <f t="shared" si="19"/>
         <v>4.9998299999999993</v>
       </c>
-      <c r="T32" s="34">
+      <c r="T32" s="52">
         <f t="shared" si="19"/>
         <v>1.4244120000000002</v>
       </c>
-      <c r="U32" s="34">
+      <c r="U32" s="52">
         <f t="shared" si="19"/>
         <v>1.4280090000000001</v>
       </c>
-      <c r="V32" s="34">
+      <c r="V32" s="52">
         <f t="shared" si="19"/>
         <v>9.2011260000000004</v>
       </c>
-      <c r="W32" s="34">
+      <c r="W32" s="52">
         <f t="shared" si="19"/>
         <v>1.8560520000000003</v>
       </c>
-      <c r="X32" s="34">
+      <c r="X32" s="52">
         <f t="shared" si="19"/>
         <v>3.3847770000000006</v>
       </c>
-      <c r="Y32" s="34">
+      <c r="Y32" s="52">
         <f t="shared" si="19"/>
         <v>3.7768500000000009</v>
       </c>
-      <c r="Z32" s="34">
+      <c r="Z32" s="52">
         <f t="shared" si="19"/>
         <v>1.2877260000000001</v>
       </c>
-      <c r="AA32" s="34">
+      <c r="AA32" s="52">
         <f t="shared" si="19"/>
         <v>3.6905220000000001</v>
       </c>
-      <c r="AB32" s="34">
+      <c r="AB32" s="52">
         <f t="shared" si="19"/>
         <v>0.48559500000000005</v>
       </c>
-      <c r="AC32" s="34">
+      <c r="AC32" s="52">
         <f t="shared" si="19"/>
         <v>2.0502899999999999</v>
       </c>
-      <c r="AD32" s="34">
+      <c r="AD32" s="52">
         <f t="shared" si="19"/>
         <v>1.1726220000000001</v>
       </c>
-      <c r="AE32" s="34">
+      <c r="AE32" s="52">
         <f t="shared" si="19"/>
         <v>0.83450400000000013</v>
       </c>
-      <c r="AF32" s="34">
+      <c r="AF32" s="52">
         <f t="shared" si="19"/>
         <v>1.7553360000000002</v>
       </c>
-      <c r="AG32" s="34">
+      <c r="AG32" s="52">
         <f t="shared" si="19"/>
         <v>2.5898400000000001</v>
       </c>
-      <c r="AH32" s="34">
+      <c r="AH32" s="52">
         <f t="shared" si="19"/>
         <v>3.7264920000000004</v>
       </c>
@@ -6335,7 +6337,7 @@
     </row>
     <row r="33" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="32"/>
-      <c r="C33" s="51"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="32"/>
       <c r="E33" s="33">
         <v>0</v>
@@ -6344,85 +6346,85 @@
         <v>96</v>
       </c>
       <c r="G33" s="32"/>
-      <c r="H33" s="53">
+      <c r="H33" s="52">
         <v>5</v>
       </c>
-      <c r="I33" s="53">
+      <c r="I33" s="52">
         <v>5</v>
       </c>
-      <c r="J33" s="53">
+      <c r="J33" s="52">
         <v>5</v>
       </c>
-      <c r="K33" s="53">
+      <c r="K33" s="52">
         <v>5</v>
       </c>
-      <c r="L33" s="53">
+      <c r="L33" s="52">
         <v>5</v>
       </c>
-      <c r="M33" s="53">
+      <c r="M33" s="52">
         <v>5</v>
       </c>
-      <c r="N33" s="53">
+      <c r="N33" s="52">
         <v>5</v>
       </c>
-      <c r="O33" s="53">
+      <c r="O33" s="52">
         <v>5</v>
       </c>
-      <c r="P33" s="53">
+      <c r="P33" s="52">
         <v>5</v>
       </c>
-      <c r="Q33" s="53">
+      <c r="Q33" s="52">
         <v>5</v>
       </c>
-      <c r="R33" s="53">
+      <c r="R33" s="52">
         <v>5</v>
       </c>
-      <c r="S33" s="53">
+      <c r="S33" s="52">
         <v>5</v>
       </c>
-      <c r="T33" s="53">
+      <c r="T33" s="52">
         <v>5</v>
       </c>
-      <c r="U33" s="53">
+      <c r="U33" s="52">
         <v>5</v>
       </c>
-      <c r="V33" s="53">
+      <c r="V33" s="52">
         <v>5</v>
       </c>
-      <c r="W33" s="53">
+      <c r="W33" s="52">
         <v>5</v>
       </c>
-      <c r="X33" s="53">
+      <c r="X33" s="52">
         <v>5</v>
       </c>
-      <c r="Y33" s="53">
+      <c r="Y33" s="52">
         <v>5</v>
       </c>
-      <c r="Z33" s="53">
+      <c r="Z33" s="52">
         <v>5</v>
       </c>
-      <c r="AA33" s="53">
+      <c r="AA33" s="52">
         <v>5</v>
       </c>
-      <c r="AB33" s="53">
+      <c r="AB33" s="52">
         <v>5</v>
       </c>
-      <c r="AC33" s="53">
+      <c r="AC33" s="52">
         <v>5</v>
       </c>
-      <c r="AD33" s="53">
+      <c r="AD33" s="52">
         <v>5</v>
       </c>
-      <c r="AE33" s="53">
+      <c r="AE33" s="52">
         <v>5</v>
       </c>
-      <c r="AF33" s="53">
+      <c r="AF33" s="52">
         <v>5</v>
       </c>
-      <c r="AG33" s="53">
+      <c r="AG33" s="52">
         <v>5</v>
       </c>
-      <c r="AH33" s="53">
+      <c r="AH33" s="52">
         <v>5</v>
       </c>
       <c r="AI33" s="32"/>
@@ -6430,7 +6432,7 @@
     <row r="34" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="29"/>
       <c r="C34" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>9</v>
@@ -6438,87 +6440,87 @@
       <c r="E34" s="31">
         <v>2018</v>
       </c>
-      <c r="F34" s="55"/>
+      <c r="F34" s="54"/>
       <c r="G34" s="29"/>
-      <c r="H34" s="54">
+      <c r="H34" s="53">
         <v>1</v>
       </c>
-      <c r="I34" s="54">
+      <c r="I34" s="53">
         <v>1</v>
       </c>
-      <c r="J34" s="54">
+      <c r="J34" s="53">
         <v>1</v>
       </c>
-      <c r="K34" s="54">
+      <c r="K34" s="53">
         <v>1</v>
       </c>
-      <c r="L34" s="54">
+      <c r="L34" s="53">
         <v>1</v>
       </c>
-      <c r="M34" s="54">
+      <c r="M34" s="53">
         <v>1</v>
       </c>
-      <c r="N34" s="54">
+      <c r="N34" s="53">
         <v>1</v>
       </c>
-      <c r="O34" s="54">
+      <c r="O34" s="53">
         <v>1</v>
       </c>
-      <c r="P34" s="54">
+      <c r="P34" s="53">
         <v>1</v>
       </c>
-      <c r="Q34" s="54">
+      <c r="Q34" s="53">
         <v>1</v>
       </c>
-      <c r="R34" s="54">
+      <c r="R34" s="53">
         <v>1</v>
       </c>
-      <c r="S34" s="54">
+      <c r="S34" s="53">
         <v>1</v>
       </c>
-      <c r="T34" s="54">
+      <c r="T34" s="53">
         <v>1</v>
       </c>
-      <c r="U34" s="54">
+      <c r="U34" s="53">
         <v>1</v>
       </c>
-      <c r="V34" s="54">
+      <c r="V34" s="53">
         <v>1</v>
       </c>
-      <c r="W34" s="54">
+      <c r="W34" s="53">
         <v>1</v>
       </c>
-      <c r="X34" s="54">
+      <c r="X34" s="53">
         <v>1</v>
       </c>
-      <c r="Y34" s="54">
+      <c r="Y34" s="53">
         <v>1</v>
       </c>
-      <c r="Z34" s="54">
+      <c r="Z34" s="53">
         <v>1</v>
       </c>
-      <c r="AA34" s="54">
+      <c r="AA34" s="53">
         <v>1</v>
       </c>
-      <c r="AB34" s="54">
+      <c r="AB34" s="53">
         <v>1</v>
       </c>
-      <c r="AC34" s="54">
+      <c r="AC34" s="53">
         <v>1</v>
       </c>
-      <c r="AD34" s="54">
+      <c r="AD34" s="53">
         <v>1</v>
       </c>
-      <c r="AE34" s="54">
+      <c r="AE34" s="53">
         <v>1</v>
       </c>
-      <c r="AF34" s="54">
+      <c r="AF34" s="53">
         <v>1</v>
       </c>
-      <c r="AG34" s="54">
+      <c r="AG34" s="53">
         <v>1</v>
       </c>
-      <c r="AH34" s="54">
+      <c r="AH34" s="53">
         <v>1</v>
       </c>
       <c r="AI34" s="32"/>
@@ -6530,33 +6532,33 @@
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
       <c r="G35" s="32"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="49"/>
-      <c r="V35" s="49"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
-      <c r="Z35" s="49"/>
-      <c r="AA35" s="49"/>
-      <c r="AB35" s="49"/>
-      <c r="AC35" s="49"/>
-      <c r="AD35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AF35" s="49"/>
-      <c r="AG35" s="49"/>
-      <c r="AH35" s="49"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
+      <c r="Z35" s="52"/>
+      <c r="AA35" s="52"/>
+      <c r="AB35" s="52"/>
+      <c r="AC35" s="52"/>
+      <c r="AD35" s="52"/>
+      <c r="AE35" s="52"/>
+      <c r="AF35" s="52"/>
+      <c r="AG35" s="52"/>
+      <c r="AH35" s="52"/>
       <c r="AI35" s="32"/>
     </row>
     <row r="36" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -6566,77 +6568,68 @@
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
-      <c r="H36" s="34">
-        <f>H24-H23</f>
-        <v>19.581607499999997</v>
-      </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
-      <c r="AB36" s="34"/>
-      <c r="AC36" s="34"/>
-      <c r="AD36" s="34"/>
-      <c r="AE36" s="34"/>
-      <c r="AF36" s="34"/>
-      <c r="AG36" s="34"/>
-      <c r="AH36" s="34"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="52"/>
+      <c r="S36" s="52"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="52"/>
+      <c r="V36" s="52"/>
+      <c r="W36" s="52"/>
+      <c r="X36" s="52"/>
+      <c r="Y36" s="52"/>
+      <c r="Z36" s="52"/>
+      <c r="AA36" s="52"/>
+      <c r="AB36" s="52"/>
+      <c r="AC36" s="52"/>
+      <c r="AD36" s="52"/>
+      <c r="AE36" s="52"/>
+      <c r="AF36" s="52"/>
+      <c r="AG36" s="52"/>
+      <c r="AH36" s="52"/>
       <c r="AI36" s="32"/>
     </row>
     <row r="37" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="26">
-        <f>H36/4</f>
-        <v>4.8954018749999992</v>
-      </c>
+      <c r="H37" s="55"/>
       <c r="I37" s="56"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-      <c r="AA37" s="26"/>
-      <c r="AB37" s="26"/>
-      <c r="AC37" s="26"/>
-      <c r="AD37" s="26"/>
-      <c r="AE37" s="26"/>
-      <c r="AF37" s="26"/>
-      <c r="AG37" s="26"/>
-      <c r="AH37" s="26"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="55"/>
+      <c r="U37" s="55"/>
+      <c r="V37" s="55"/>
+      <c r="W37" s="55"/>
+      <c r="X37" s="55"/>
+      <c r="Y37" s="55"/>
+      <c r="Z37" s="55"/>
+      <c r="AA37" s="55"/>
+      <c r="AB37" s="55"/>
+      <c r="AC37" s="55"/>
+      <c r="AD37" s="55"/>
+      <c r="AE37" s="55"/>
+      <c r="AF37" s="55"/>
+      <c r="AG37" s="55"/>
+      <c r="AH37" s="55"/>
       <c r="AI37" s="19"/>
     </row>
     <row r="38" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="52"/>
-      <c r="H38" s="26">
-        <f>H37+H23</f>
-        <v>19.958176874999999</v>
-      </c>
+      <c r="B38" s="51"/>
+      <c r="H38" s="26"/>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
@@ -6666,7 +6659,7 @@
       <c r="AI38" s="19"/>
     </row>
     <row r="39" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="52"/>
+      <c r="B39" s="51"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
       <c r="J39" s="26"/>
@@ -6697,13 +6690,13 @@
       <c r="AI39" s="35"/>
     </row>
     <row r="40" spans="1:56" ht="21" x14ac:dyDescent="0.4">
-      <c r="B40" s="52"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
       <c r="G40" s="37" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
@@ -6737,8 +6730,8 @@
       <c r="AK40" s="27"/>
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="B41" s="52"/>
-      <c r="C41" s="27"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="59"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
@@ -6856,8 +6849,8 @@
       <c r="AK41" s="27"/>
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="B42" s="52"/>
-      <c r="C42" s="27"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="59"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
@@ -6977,8 +6970,8 @@
       <c r="AK42" s="27"/>
     </row>
     <row r="43" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="B43" s="52"/>
-      <c r="C43" s="27"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="59"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
@@ -7098,8 +7091,8 @@
       <c r="AK43" s="27"/>
     </row>
     <row r="44" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="B44" s="52"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27"/>
@@ -7219,8 +7212,8 @@
       <c r="AK44" s="27"/>
     </row>
     <row r="45" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="B45" s="52"/>
-      <c r="C45" s="27"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="27"/>
@@ -7341,7 +7334,7 @@
     </row>
     <row r="46" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A46" s="27"/>
-      <c r="B46" s="52"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
@@ -7399,7 +7392,7 @@
     </row>
     <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" s="27"/>
-      <c r="B47" s="52"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -7457,7 +7450,7 @@
     </row>
     <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" s="27"/>
-      <c r="B48" s="51"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
@@ -7515,7 +7508,7 @@
     </row>
     <row r="49" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
-      <c r="B49" s="51"/>
+      <c r="B49" s="50"/>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -7573,11 +7566,11 @@
     </row>
     <row r="50" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="27"/>
-      <c r="B50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="50" t="s">
+      <c r="B50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="49" t="s">
         <v>136</v>
       </c>
       <c r="H50" s="39"/>
@@ -7632,10 +7625,10 @@
     </row>
     <row r="51" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="27"/>
-      <c r="B51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
+      <c r="B51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
       <c r="G51" s="40" t="s">
         <v>107</v>
       </c>
@@ -7745,10 +7738,10 @@
     </row>
     <row r="52" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="27"/>
-      <c r="B52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="41" t="s">
         <v>108</v>
       </c>
@@ -7804,10 +7797,10 @@
     </row>
     <row r="53" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A53" s="27"/>
-      <c r="B53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
+      <c r="B53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
       <c r="G53" s="39" t="s">
         <v>109</v>
       </c>
@@ -7917,10 +7910,10 @@
     </row>
     <row r="54" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="27"/>
-      <c r="B54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
+      <c r="B54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
       <c r="G54" s="41" t="s">
         <v>110</v>
       </c>
@@ -7976,9 +7969,9 @@
     </row>
     <row r="55" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A55" s="27"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="51"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
       <c r="G55" s="39" t="s">
         <v>111</v>
       </c>
@@ -8088,9 +8081,9 @@
     </row>
     <row r="56" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="51"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
       <c r="G56" s="39" t="s">
         <v>112</v>
       </c>
@@ -8200,9 +8193,9 @@
     </row>
     <row r="57" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A57" s="27"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="51"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
       <c r="G57" s="39" t="s">
         <v>113</v>
       </c>
@@ -8312,9 +8305,9 @@
     </row>
     <row r="58" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A58" s="27"/>
-      <c r="D58" s="51"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="51"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
       <c r="G58" s="39" t="s">
         <v>114</v>
       </c>
@@ -8424,9 +8417,9 @@
     </row>
     <row r="59" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A59" s="27"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="51"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
       <c r="G59" s="39" t="s">
         <v>115</v>
       </c>
@@ -8536,9 +8529,9 @@
     </row>
     <row r="60" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A60" s="27"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
       <c r="G60" s="39" t="s">
         <v>116</v>
       </c>
@@ -8648,9 +8641,9 @@
     </row>
     <row r="61" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A61" s="27"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="51"/>
-      <c r="F61" s="51"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
       <c r="G61" s="39" t="s">
         <v>117</v>
       </c>
@@ -8760,9 +8753,9 @@
     </row>
     <row r="62" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A62" s="27"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
       <c r="G62" s="39" t="s">
         <v>118</v>
       </c>
@@ -8872,9 +8865,9 @@
     </row>
     <row r="63" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A63" s="27"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="51"/>
-      <c r="F63" s="51"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
       <c r="G63" s="39" t="s">
         <v>119</v>
       </c>
@@ -8984,9 +8977,9 @@
     </row>
     <row r="64" spans="1:56" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="27"/>
-      <c r="D64" s="51"/>
-      <c r="E64" s="51"/>
-      <c r="F64" s="51"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
       <c r="G64" s="41" t="s">
         <v>120</v>
       </c>
@@ -9042,9 +9035,9 @@
     </row>
     <row r="65" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="50"/>
       <c r="G65" s="39" t="s">
         <v>121</v>
       </c>
@@ -9154,9 +9147,9 @@
     </row>
     <row r="66" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="27"/>
-      <c r="D66" s="51"/>
-      <c r="E66" s="51"/>
-      <c r="F66" s="51"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
       <c r="G66" s="39" t="s">
         <v>122</v>
       </c>
@@ -9266,9 +9259,9 @@
     </row>
     <row r="67" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="27"/>
-      <c r="D67" s="51"/>
-      <c r="E67" s="51"/>
-      <c r="F67" s="51"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
       <c r="G67" s="39" t="s">
         <v>123</v>
       </c>
@@ -9378,9 +9371,9 @@
     </row>
     <row r="68" spans="1:56" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="27"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="51"/>
-      <c r="F68" s="51"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
       <c r="G68" s="41" t="s">
         <v>124</v>
       </c>
@@ -9436,9 +9429,9 @@
     </row>
     <row r="69" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27"/>
-      <c r="D69" s="51"/>
-      <c r="E69" s="51"/>
-      <c r="F69" s="51"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
       <c r="G69" s="39" t="s">
         <v>125</v>
       </c>
@@ -9547,9 +9540,9 @@
       <c r="BD69" s="27"/>
     </row>
     <row r="70" spans="1:56" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
-      <c r="F70" s="51"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
       <c r="G70" s="41" t="s">
         <v>126</v>
       </c>
@@ -9582,9 +9575,9 @@
       <c r="AH70" s="42"/>
     </row>
     <row r="71" spans="1:56" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="50"/>
+      <c r="F71" s="50"/>
       <c r="G71" s="39" t="s">
         <v>127</v>
       </c>
@@ -9672,9 +9665,9 @@
     </row>
     <row r="72" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="27"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
       <c r="G72" s="39" t="s">
         <v>128</v>
       </c>
@@ -9784,9 +9777,9 @@
     </row>
     <row r="73" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="27"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
-      <c r="F73" s="51"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
       <c r="G73" s="39" t="s">
         <v>129</v>
       </c>
@@ -9896,9 +9889,9 @@
     </row>
     <row r="74" spans="1:56" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="27"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="50"/>
+      <c r="F74" s="50"/>
       <c r="G74" s="41" t="s">
         <v>130</v>
       </c>
@@ -9954,9 +9947,9 @@
     </row>
     <row r="75" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="27"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="51"/>
-      <c r="F75" s="51"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
       <c r="G75" s="39" t="s">
         <v>131</v>
       </c>
@@ -10066,9 +10059,9 @@
     </row>
     <row r="76" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="27"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
       <c r="G76" s="39" t="s">
         <v>132</v>
       </c>
@@ -10178,9 +10171,9 @@
     </row>
     <row r="77" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="27"/>
-      <c r="D77" s="51"/>
-      <c r="E77" s="51"/>
-      <c r="F77" s="51"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="50"/>
+      <c r="F77" s="50"/>
       <c r="G77" s="39" t="s">
         <v>133</v>
       </c>
@@ -10290,13 +10283,13 @@
     </row>
     <row r="78" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27"/>
-      <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="51"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
       <c r="G78" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H78" s="44">
+      <c r="H78" s="43">
         <v>21.648000000000003</v>
       </c>
       <c r="I78" s="45">
@@ -10402,9 +10395,9 @@
     </row>
     <row r="79" spans="1:56" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="27"/>
-      <c r="D79" s="51"/>
-      <c r="E79" s="51"/>
-      <c r="F79" s="51"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
       <c r="G79" s="39" t="s">
         <v>135</v>
       </c>
@@ -10516,9 +10509,9 @@
       <c r="A80" s="27"/>
       <c r="B80" s="27"/>
       <c r="C80" s="27"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="51"/>
-      <c r="F80" s="51"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="50"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
       <c r="I80" s="27"/>
@@ -10635,8 +10628,13 @@
       <c r="D82" s="27"/>
       <c r="E82" s="27"/>
       <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
+      <c r="G82" s="27">
+        <v>2020</v>
+      </c>
+      <c r="H82" s="58">
+        <f>2.043+H78</f>
+        <v>23.691000000000003</v>
+      </c>
       <c r="I82" s="27"/>
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>

</xml_diff>

<commit_message>
Modify max stock for HGTs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E141F-9CA2-43DA-9D3C-B6098A24960F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55913A9-9C93-4452-B5E3-A623B1922F6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,7 +1464,7 @@
     <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1545,7 +1545,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="68" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -3204,8 +3203,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5749,113 +5748,113 @@
       <c r="G28" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="H28" s="57">
-        <f>H45*1.1</f>
-        <v>23.812800000000006</v>
+      <c r="H28" s="52">
+        <f>H45*1.16</f>
+        <v>25.111680000000003</v>
       </c>
       <c r="I28" s="52">
-        <f>I45*1.1</f>
-        <v>0.42900000000000005</v>
+        <f t="shared" ref="I28:AH28" si="15">I45*1.16</f>
+        <v>0.45239999999999997</v>
       </c>
       <c r="J28" s="52">
-        <f t="shared" ref="I28:AH28" si="15">J45*1.1</f>
-        <v>4.2713000000000001</v>
+        <f t="shared" si="15"/>
+        <v>4.5042799999999996</v>
       </c>
       <c r="K28" s="52">
         <f t="shared" si="15"/>
-        <v>1.2232000000000003</v>
+        <v>1.28992</v>
       </c>
       <c r="L28" s="52">
         <f t="shared" si="15"/>
-        <v>0.7843</v>
+        <v>0.82707999999999993</v>
       </c>
       <c r="M28" s="52">
         <f t="shared" si="15"/>
-        <v>0.50050000000000006</v>
+        <v>0.52779999999999994</v>
       </c>
       <c r="N28" s="52">
         <f t="shared" si="15"/>
-        <v>0.30360000000000004</v>
+        <v>0.32016</v>
       </c>
       <c r="O28" s="52">
         <f t="shared" si="15"/>
-        <v>0.67870000000000008</v>
+        <v>0.71571999999999991</v>
       </c>
       <c r="P28" s="52">
         <f t="shared" si="15"/>
-        <v>1.5664</v>
+        <v>1.6518399999999998</v>
       </c>
       <c r="Q28" s="52">
         <f t="shared" si="15"/>
-        <v>0.35530000000000006</v>
+        <v>0.37467999999999996</v>
       </c>
       <c r="R28" s="52">
         <f t="shared" si="15"/>
-        <v>0.34760000000000002</v>
+        <v>0.36656</v>
       </c>
       <c r="S28" s="52">
         <f t="shared" si="15"/>
-        <v>1.5289999999999999</v>
+        <v>1.6123999999999998</v>
       </c>
       <c r="T28" s="52">
         <f t="shared" si="15"/>
-        <v>0.43560000000000004</v>
+        <v>0.45935999999999999</v>
       </c>
       <c r="U28" s="52">
         <f t="shared" si="15"/>
-        <v>0.43670000000000003</v>
+        <v>0.46051999999999998</v>
       </c>
       <c r="V28" s="52">
         <f t="shared" si="15"/>
-        <v>2.8138000000000001</v>
+        <v>2.9672799999999997</v>
       </c>
       <c r="W28" s="52">
         <f t="shared" si="15"/>
-        <v>0.5676000000000001</v>
+        <v>0.59855999999999998</v>
       </c>
       <c r="X28" s="52">
         <f t="shared" si="15"/>
-        <v>1.0351000000000001</v>
+        <v>1.0915599999999999</v>
       </c>
       <c r="Y28" s="52">
         <f t="shared" si="15"/>
-        <v>1.1550000000000002</v>
+        <v>1.218</v>
       </c>
       <c r="Z28" s="52">
         <f t="shared" si="15"/>
-        <v>0.39380000000000004</v>
+        <v>0.41527999999999993</v>
       </c>
       <c r="AA28" s="52">
         <f t="shared" si="15"/>
-        <v>1.1286</v>
+        <v>1.1901599999999999</v>
       </c>
       <c r="AB28" s="52">
         <f t="shared" si="15"/>
-        <v>0.14850000000000002</v>
+        <v>0.15659999999999999</v>
       </c>
       <c r="AC28" s="52">
         <f t="shared" si="15"/>
-        <v>0.627</v>
+        <v>0.6611999999999999</v>
       </c>
       <c r="AD28" s="52">
         <f t="shared" si="15"/>
-        <v>0.35860000000000003</v>
+        <v>0.37816</v>
       </c>
       <c r="AE28" s="52">
         <f t="shared" si="15"/>
-        <v>0.25520000000000004</v>
+        <v>0.26911999999999997</v>
       </c>
       <c r="AF28" s="52">
         <f t="shared" si="15"/>
-        <v>0.53680000000000005</v>
+        <v>0.56607999999999992</v>
       </c>
       <c r="AG28" s="52">
         <f t="shared" si="15"/>
-        <v>0.79200000000000004</v>
+        <v>0.83519999999999994</v>
       </c>
       <c r="AH28" s="52">
         <f t="shared" si="15"/>
-        <v>1.1396000000000002</v>
+        <v>1.2017599999999999</v>
       </c>
       <c r="AI28" s="32"/>
     </row>
@@ -5868,113 +5867,113 @@
         <v>96</v>
       </c>
       <c r="G29" s="32"/>
-      <c r="H29" s="57">
-        <f>H28*1.05</f>
-        <v>25.003440000000008</v>
+      <c r="H29" s="52">
+        <f>H28</f>
+        <v>25.111680000000003</v>
       </c>
       <c r="I29" s="52">
         <f t="shared" ref="I29:AH29" si="16">I28</f>
-        <v>0.42900000000000005</v>
+        <v>0.45239999999999997</v>
       </c>
       <c r="J29" s="52">
         <f t="shared" si="16"/>
-        <v>4.2713000000000001</v>
+        <v>4.5042799999999996</v>
       </c>
       <c r="K29" s="52">
         <f t="shared" si="16"/>
-        <v>1.2232000000000003</v>
+        <v>1.28992</v>
       </c>
       <c r="L29" s="52">
         <f t="shared" si="16"/>
-        <v>0.7843</v>
+        <v>0.82707999999999993</v>
       </c>
       <c r="M29" s="52">
         <f t="shared" si="16"/>
-        <v>0.50050000000000006</v>
+        <v>0.52779999999999994</v>
       </c>
       <c r="N29" s="52">
         <f t="shared" si="16"/>
-        <v>0.30360000000000004</v>
+        <v>0.32016</v>
       </c>
       <c r="O29" s="52">
         <f t="shared" si="16"/>
-        <v>0.67870000000000008</v>
+        <v>0.71571999999999991</v>
       </c>
       <c r="P29" s="52">
         <f t="shared" si="16"/>
-        <v>1.5664</v>
+        <v>1.6518399999999998</v>
       </c>
       <c r="Q29" s="52">
         <f t="shared" si="16"/>
-        <v>0.35530000000000006</v>
+        <v>0.37467999999999996</v>
       </c>
       <c r="R29" s="52">
         <f t="shared" si="16"/>
-        <v>0.34760000000000002</v>
+        <v>0.36656</v>
       </c>
       <c r="S29" s="52">
         <f t="shared" si="16"/>
-        <v>1.5289999999999999</v>
+        <v>1.6123999999999998</v>
       </c>
       <c r="T29" s="52">
         <f t="shared" si="16"/>
-        <v>0.43560000000000004</v>
+        <v>0.45935999999999999</v>
       </c>
       <c r="U29" s="52">
         <f t="shared" si="16"/>
-        <v>0.43670000000000003</v>
+        <v>0.46051999999999998</v>
       </c>
       <c r="V29" s="52">
         <f t="shared" si="16"/>
-        <v>2.8138000000000001</v>
+        <v>2.9672799999999997</v>
       </c>
       <c r="W29" s="52">
         <f t="shared" si="16"/>
-        <v>0.5676000000000001</v>
+        <v>0.59855999999999998</v>
       </c>
       <c r="X29" s="52">
         <f t="shared" si="16"/>
-        <v>1.0351000000000001</v>
+        <v>1.0915599999999999</v>
       </c>
       <c r="Y29" s="52">
         <f t="shared" si="16"/>
-        <v>1.1550000000000002</v>
+        <v>1.218</v>
       </c>
       <c r="Z29" s="52">
         <f t="shared" si="16"/>
-        <v>0.39380000000000004</v>
+        <v>0.41527999999999993</v>
       </c>
       <c r="AA29" s="52">
         <f t="shared" si="16"/>
-        <v>1.1286</v>
+        <v>1.1901599999999999</v>
       </c>
       <c r="AB29" s="52">
         <f t="shared" si="16"/>
-        <v>0.14850000000000002</v>
+        <v>0.15659999999999999</v>
       </c>
       <c r="AC29" s="52">
         <f t="shared" si="16"/>
-        <v>0.627</v>
+        <v>0.6611999999999999</v>
       </c>
       <c r="AD29" s="52">
         <f t="shared" si="16"/>
-        <v>0.35860000000000003</v>
+        <v>0.37816</v>
       </c>
       <c r="AE29" s="52">
         <f t="shared" si="16"/>
-        <v>0.25520000000000004</v>
+        <v>0.26911999999999997</v>
       </c>
       <c r="AF29" s="52">
         <f t="shared" si="16"/>
-        <v>0.53680000000000005</v>
+        <v>0.56607999999999992</v>
       </c>
       <c r="AG29" s="52">
         <f t="shared" si="16"/>
-        <v>0.79200000000000004</v>
+        <v>0.83519999999999994</v>
       </c>
       <c r="AH29" s="52">
         <f t="shared" si="16"/>
-        <v>1.1396000000000002</v>
+        <v>1.2017599999999999</v>
       </c>
       <c r="AI29" s="32"/>
     </row>
@@ -5987,113 +5986,113 @@
         <v>96</v>
       </c>
       <c r="G30" s="32"/>
-      <c r="H30" s="57">
+      <c r="H30" s="52">
         <f>H29*1.25</f>
-        <v>31.254300000000011</v>
+        <v>31.389600000000005</v>
       </c>
       <c r="I30" s="52">
-        <f t="shared" ref="I30:AH30" si="17">I29*1.3</f>
-        <v>0.55770000000000008</v>
+        <f t="shared" ref="I30:AH30" si="17">I29*1.25</f>
+        <v>0.5655</v>
       </c>
       <c r="J30" s="52">
         <f t="shared" si="17"/>
-        <v>5.5526900000000001</v>
+        <v>5.63035</v>
       </c>
       <c r="K30" s="52">
         <f t="shared" si="17"/>
-        <v>1.5901600000000005</v>
+        <v>1.6124000000000001</v>
       </c>
       <c r="L30" s="52">
         <f t="shared" si="17"/>
-        <v>1.01959</v>
+        <v>1.0338499999999999</v>
       </c>
       <c r="M30" s="52">
         <f t="shared" si="17"/>
-        <v>0.65065000000000006</v>
+        <v>0.65974999999999995</v>
       </c>
       <c r="N30" s="52">
         <f t="shared" si="17"/>
-        <v>0.39468000000000009</v>
+        <v>0.4002</v>
       </c>
       <c r="O30" s="52">
         <f t="shared" si="17"/>
-        <v>0.88231000000000015</v>
+        <v>0.89464999999999995</v>
       </c>
       <c r="P30" s="52">
         <f t="shared" si="17"/>
-        <v>2.0363199999999999</v>
+        <v>2.0647999999999995</v>
       </c>
       <c r="Q30" s="52">
         <f t="shared" si="17"/>
-        <v>0.46189000000000008</v>
+        <v>0.46834999999999993</v>
       </c>
       <c r="R30" s="52">
         <f t="shared" si="17"/>
-        <v>0.45188000000000006</v>
+        <v>0.4582</v>
       </c>
       <c r="S30" s="52">
         <f t="shared" si="17"/>
-        <v>1.9877</v>
+        <v>2.0154999999999998</v>
       </c>
       <c r="T30" s="52">
         <f t="shared" si="17"/>
-        <v>0.56628000000000012</v>
+        <v>0.57420000000000004</v>
       </c>
       <c r="U30" s="52">
         <f t="shared" si="17"/>
-        <v>0.56771000000000005</v>
+        <v>0.57565</v>
       </c>
       <c r="V30" s="52">
         <f t="shared" si="17"/>
-        <v>3.6579400000000004</v>
+        <v>3.7090999999999994</v>
       </c>
       <c r="W30" s="52">
         <f t="shared" si="17"/>
-        <v>0.7378800000000002</v>
+        <v>0.74819999999999998</v>
       </c>
       <c r="X30" s="52">
         <f t="shared" si="17"/>
-        <v>1.3456300000000003</v>
+        <v>1.3644499999999997</v>
       </c>
       <c r="Y30" s="52">
         <f t="shared" si="17"/>
-        <v>1.5015000000000003</v>
+        <v>1.5225</v>
       </c>
       <c r="Z30" s="52">
         <f t="shared" si="17"/>
-        <v>0.51194000000000006</v>
+        <v>0.51909999999999989</v>
       </c>
       <c r="AA30" s="52">
         <f t="shared" si="17"/>
-        <v>1.4671800000000002</v>
+        <v>1.4876999999999998</v>
       </c>
       <c r="AB30" s="52">
         <f t="shared" si="17"/>
-        <v>0.19305000000000003</v>
+        <v>0.19574999999999998</v>
       </c>
       <c r="AC30" s="52">
         <f t="shared" si="17"/>
-        <v>0.81510000000000005</v>
+        <v>0.8264999999999999</v>
       </c>
       <c r="AD30" s="52">
         <f t="shared" si="17"/>
-        <v>0.46618000000000004</v>
+        <v>0.47270000000000001</v>
       </c>
       <c r="AE30" s="52">
         <f t="shared" si="17"/>
-        <v>0.33176000000000005</v>
+        <v>0.33639999999999998</v>
       </c>
       <c r="AF30" s="52">
         <f t="shared" si="17"/>
-        <v>0.69784000000000013</v>
+        <v>0.7075999999999999</v>
       </c>
       <c r="AG30" s="52">
         <f t="shared" si="17"/>
-        <v>1.0296000000000001</v>
+        <v>1.044</v>
       </c>
       <c r="AH30" s="52">
         <f t="shared" si="17"/>
-        <v>1.4814800000000004</v>
+        <v>1.5022</v>
       </c>
       <c r="AI30" s="32"/>
     </row>
@@ -6106,113 +6105,113 @@
         <v>96</v>
       </c>
       <c r="G31" s="32"/>
-      <c r="H31" s="57">
+      <c r="H31" s="52">
         <f>H30*1.9</f>
-        <v>59.383170000000021</v>
+        <v>59.640240000000006</v>
       </c>
       <c r="I31" s="52">
         <f t="shared" ref="I31:AH31" si="18">I30*1.9</f>
-        <v>1.0596300000000001</v>
+        <v>1.0744499999999999</v>
       </c>
       <c r="J31" s="52">
         <f t="shared" si="18"/>
-        <v>10.550110999999999</v>
+        <v>10.697664999999999</v>
       </c>
       <c r="K31" s="52">
         <f t="shared" si="18"/>
-        <v>3.0213040000000007</v>
+        <v>3.0635599999999998</v>
       </c>
       <c r="L31" s="52">
         <f t="shared" si="18"/>
-        <v>1.9372209999999999</v>
+        <v>1.9643149999999998</v>
       </c>
       <c r="M31" s="52">
         <f t="shared" si="18"/>
-        <v>1.236235</v>
+        <v>1.2535249999999998</v>
       </c>
       <c r="N31" s="52">
         <f t="shared" si="18"/>
-        <v>0.74989200000000011</v>
+        <v>0.76037999999999994</v>
       </c>
       <c r="O31" s="52">
         <f t="shared" si="18"/>
-        <v>1.6763890000000001</v>
+        <v>1.6998349999999998</v>
       </c>
       <c r="P31" s="52">
         <f t="shared" si="18"/>
-        <v>3.8690079999999996</v>
+        <v>3.9231199999999991</v>
       </c>
       <c r="Q31" s="52">
         <f t="shared" si="18"/>
-        <v>0.87759100000000012</v>
+        <v>0.8898649999999998</v>
       </c>
       <c r="R31" s="52">
         <f t="shared" si="18"/>
-        <v>0.85857200000000011</v>
+        <v>0.87057999999999991</v>
       </c>
       <c r="S31" s="52">
         <f t="shared" si="18"/>
-        <v>3.7766299999999999</v>
+        <v>3.8294499999999996</v>
       </c>
       <c r="T31" s="52">
         <f t="shared" si="18"/>
-        <v>1.0759320000000001</v>
+        <v>1.0909800000000001</v>
       </c>
       <c r="U31" s="52">
         <f t="shared" si="18"/>
-        <v>1.078649</v>
+        <v>1.0937349999999999</v>
       </c>
       <c r="V31" s="52">
         <f t="shared" si="18"/>
-        <v>6.9500860000000007</v>
+        <v>7.0472899999999985</v>
       </c>
       <c r="W31" s="52">
         <f t="shared" si="18"/>
-        <v>1.4019720000000002</v>
+        <v>1.4215799999999998</v>
       </c>
       <c r="X31" s="52">
         <f t="shared" si="18"/>
-        <v>2.5566970000000007</v>
+        <v>2.5924549999999993</v>
       </c>
       <c r="Y31" s="52">
         <f t="shared" si="18"/>
-        <v>2.8528500000000006</v>
+        <v>2.8927499999999999</v>
       </c>
       <c r="Z31" s="52">
         <f t="shared" si="18"/>
-        <v>0.97268600000000005</v>
+        <v>0.98628999999999978</v>
       </c>
       <c r="AA31" s="52">
         <f t="shared" si="18"/>
-        <v>2.787642</v>
+        <v>2.8266299999999993</v>
       </c>
       <c r="AB31" s="52">
         <f t="shared" si="18"/>
-        <v>0.36679500000000004</v>
+        <v>0.37192499999999995</v>
       </c>
       <c r="AC31" s="52">
         <f t="shared" si="18"/>
-        <v>1.5486900000000001</v>
+        <v>1.5703499999999997</v>
       </c>
       <c r="AD31" s="52">
         <f t="shared" si="18"/>
-        <v>0.88574200000000003</v>
+        <v>0.89812999999999998</v>
       </c>
       <c r="AE31" s="52">
         <f t="shared" si="18"/>
-        <v>0.63034400000000013</v>
+        <v>0.63915999999999995</v>
       </c>
       <c r="AF31" s="52">
         <f t="shared" si="18"/>
-        <v>1.3258960000000002</v>
+        <v>1.3444399999999996</v>
       </c>
       <c r="AG31" s="52">
         <f t="shared" si="18"/>
-        <v>1.95624</v>
+        <v>1.9836</v>
       </c>
       <c r="AH31" s="52">
         <f t="shared" si="18"/>
-        <v>2.8148120000000008</v>
+        <v>2.8541799999999999</v>
       </c>
       <c r="AI31" s="32"/>
     </row>
@@ -6227,111 +6226,111 @@
       <c r="G32" s="32"/>
       <c r="H32" s="52">
         <f>H28*3.27</f>
-        <v>77.867856000000018</v>
+        <v>82.115193600000012</v>
       </c>
       <c r="I32" s="52">
         <f t="shared" ref="I32:AH32" si="19">I28*3.27</f>
-        <v>1.4028300000000002</v>
+        <v>1.4793479999999999</v>
       </c>
       <c r="J32" s="52">
         <f t="shared" si="19"/>
-        <v>13.967151000000001</v>
+        <v>14.728995599999999</v>
       </c>
       <c r="K32" s="52">
         <f t="shared" si="19"/>
-        <v>3.999864000000001</v>
+        <v>4.2180384000000002</v>
       </c>
       <c r="L32" s="52">
         <f t="shared" si="19"/>
-        <v>2.5646610000000001</v>
+        <v>2.7045515999999998</v>
       </c>
       <c r="M32" s="52">
         <f t="shared" si="19"/>
-        <v>1.6366350000000003</v>
+        <v>1.7259059999999997</v>
       </c>
       <c r="N32" s="52">
         <f t="shared" si="19"/>
-        <v>0.9927720000000001</v>
+        <v>1.0469231999999999</v>
       </c>
       <c r="O32" s="52">
         <f t="shared" si="19"/>
-        <v>2.2193490000000002</v>
+        <v>2.3404043999999997</v>
       </c>
       <c r="P32" s="52">
         <f t="shared" si="19"/>
-        <v>5.122128</v>
+        <v>5.4015167999999996</v>
       </c>
       <c r="Q32" s="52">
         <f t="shared" si="19"/>
-        <v>1.1618310000000003</v>
+        <v>1.2252035999999999</v>
       </c>
       <c r="R32" s="52">
         <f t="shared" si="19"/>
-        <v>1.136652</v>
+        <v>1.1986512</v>
       </c>
       <c r="S32" s="52">
         <f t="shared" si="19"/>
-        <v>4.9998299999999993</v>
+        <v>5.2725479999999996</v>
       </c>
       <c r="T32" s="52">
         <f t="shared" si="19"/>
-        <v>1.4244120000000002</v>
+        <v>1.5021072</v>
       </c>
       <c r="U32" s="52">
         <f t="shared" si="19"/>
-        <v>1.4280090000000001</v>
+        <v>1.5059004</v>
       </c>
       <c r="V32" s="52">
         <f t="shared" si="19"/>
-        <v>9.2011260000000004</v>
+        <v>9.7030055999999991</v>
       </c>
       <c r="W32" s="52">
         <f t="shared" si="19"/>
-        <v>1.8560520000000003</v>
+        <v>1.9572912</v>
       </c>
       <c r="X32" s="52">
         <f t="shared" si="19"/>
-        <v>3.3847770000000006</v>
+        <v>3.5694011999999997</v>
       </c>
       <c r="Y32" s="52">
         <f t="shared" si="19"/>
-        <v>3.7768500000000009</v>
+        <v>3.9828600000000001</v>
       </c>
       <c r="Z32" s="52">
         <f t="shared" si="19"/>
-        <v>1.2877260000000001</v>
+        <v>1.3579655999999998</v>
       </c>
       <c r="AA32" s="52">
         <f t="shared" si="19"/>
-        <v>3.6905220000000001</v>
+        <v>3.8918231999999997</v>
       </c>
       <c r="AB32" s="52">
         <f t="shared" si="19"/>
-        <v>0.48559500000000005</v>
+        <v>0.51208199999999993</v>
       </c>
       <c r="AC32" s="52">
         <f t="shared" si="19"/>
-        <v>2.0502899999999999</v>
+        <v>2.1621239999999995</v>
       </c>
       <c r="AD32" s="52">
         <f t="shared" si="19"/>
-        <v>1.1726220000000001</v>
+        <v>1.2365832000000001</v>
       </c>
       <c r="AE32" s="52">
         <f t="shared" si="19"/>
-        <v>0.83450400000000013</v>
+        <v>0.88002239999999987</v>
       </c>
       <c r="AF32" s="52">
         <f t="shared" si="19"/>
-        <v>1.7553360000000002</v>
+        <v>1.8510815999999997</v>
       </c>
       <c r="AG32" s="52">
         <f t="shared" si="19"/>
-        <v>2.5898400000000001</v>
+        <v>2.7311039999999998</v>
       </c>
       <c r="AH32" s="52">
         <f t="shared" si="19"/>
-        <v>3.7264920000000004</v>
+        <v>3.9297551999999998</v>
       </c>
       <c r="AI32" s="32"/>
     </row>
@@ -6731,7 +6730,7 @@
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B41" s="51"/>
-      <c r="C41" s="59"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
@@ -6850,7 +6849,7 @@
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B42" s="51"/>
-      <c r="C42" s="59"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
@@ -6971,7 +6970,7 @@
     </row>
     <row r="43" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B43" s="51"/>
-      <c r="C43" s="59"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
@@ -7092,7 +7091,7 @@
     </row>
     <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B44" s="51"/>
-      <c r="C44" s="59"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27"/>
@@ -7213,7 +7212,7 @@
     </row>
     <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B45" s="51"/>
-      <c r="C45" s="59"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="27"/>
@@ -10628,13 +10627,8 @@
       <c r="D82" s="27"/>
       <c r="E82" s="27"/>
       <c r="F82" s="27"/>
-      <c r="G82" s="27">
-        <v>2020</v>
-      </c>
-      <c r="H82" s="58">
-        <f>2.043+H78</f>
-        <v>23.691000000000003</v>
-      </c>
+      <c r="G82" s="27"/>
+      <c r="H82" s="57"/>
       <c r="I82" s="27"/>
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>

</xml_diff>

<commit_message>
Modify Max Stock for Private Cars
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Stock.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF096424-DEBE-41F9-B530-D03072369275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32465F19-C16E-4FD4-8777-139C2B38D5D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3203,8 +3203,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:BD275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:E56"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3384,112 +3384,112 @@
         <v>97</v>
       </c>
       <c r="H7" s="54">
-        <f>H42*1.05</f>
-        <v>2228.8843500000003</v>
+        <f>H42*1.06</f>
+        <v>2250.1118200000005</v>
       </c>
       <c r="I7" s="54">
-        <f t="shared" ref="I7:AH7" si="0">I42*1.05</f>
-        <v>29.98695</v>
+        <f t="shared" ref="I7:AH7" si="0">I42*1.06</f>
+        <v>30.272539999999999</v>
       </c>
       <c r="J7" s="54">
         <f t="shared" si="0"/>
-        <v>554.76225000000022</v>
+        <v>560.04570000000012</v>
       </c>
       <c r="K7" s="54">
         <f t="shared" si="0"/>
-        <v>107.68275000000003</v>
+        <v>108.70830000000002</v>
       </c>
       <c r="L7" s="54">
         <f t="shared" si="0"/>
-        <v>48.583499999999994</v>
+        <v>49.046199999999992</v>
       </c>
       <c r="M7" s="54">
         <f t="shared" si="0"/>
-        <v>36.785699999999999</v>
+        <v>37.136040000000001</v>
       </c>
       <c r="N7" s="54">
         <f t="shared" si="0"/>
-        <v>19.214999999999996</v>
+        <v>19.398</v>
       </c>
       <c r="O7" s="54">
         <f t="shared" si="0"/>
-        <v>53.548949999999998</v>
+        <v>54.05894</v>
       </c>
       <c r="P7" s="54">
         <f t="shared" si="0"/>
-        <v>91.8309</v>
+        <v>92.705480000000009</v>
       </c>
       <c r="Q7" s="54">
         <f t="shared" si="0"/>
-        <v>36.018149999999999</v>
+        <v>36.361179999999997</v>
       </c>
       <c r="R7" s="54">
         <f t="shared" si="0"/>
-        <v>43.430099999999996</v>
+        <v>43.843719999999998</v>
       </c>
       <c r="S7" s="54">
         <f t="shared" si="0"/>
-        <v>78.821400000000011</v>
+        <v>79.572080000000014</v>
       </c>
       <c r="T7" s="54">
         <f t="shared" si="0"/>
-        <v>71.70975</v>
+        <v>72.392700000000005</v>
       </c>
       <c r="U7" s="54">
         <f t="shared" si="0"/>
-        <v>60.372900000000001</v>
+        <v>60.947879999999998</v>
       </c>
       <c r="V7" s="54">
         <f t="shared" si="0"/>
-        <v>271.39140000000003</v>
+        <v>273.97608000000002</v>
       </c>
       <c r="W7" s="54">
         <f t="shared" si="0"/>
-        <v>76.935599999999994</v>
+        <v>77.668319999999994</v>
       </c>
       <c r="X7" s="54">
         <f t="shared" si="0"/>
-        <v>92.664599999999993</v>
+        <v>93.547120000000007</v>
       </c>
       <c r="Y7" s="54">
         <f t="shared" si="0"/>
-        <v>82.989900000000006</v>
+        <v>83.780280000000005</v>
       </c>
       <c r="Z7" s="54">
         <f t="shared" si="0"/>
-        <v>60.668999999999997</v>
+        <v>61.246799999999993</v>
       </c>
       <c r="AA7" s="54">
         <f t="shared" si="0"/>
-        <v>136.81920000000005</v>
+        <v>138.12224000000003</v>
       </c>
       <c r="AB7" s="54">
         <f t="shared" si="0"/>
-        <v>15.622949999999999</v>
+        <v>15.771740000000001</v>
       </c>
       <c r="AC7" s="54">
         <f t="shared" si="0"/>
-        <v>64.41749999999999</v>
+        <v>65.030999999999992</v>
       </c>
       <c r="AD7" s="54">
         <f t="shared" si="0"/>
-        <v>34.345500000000008</v>
+        <v>34.67260000000001</v>
       </c>
       <c r="AE7" s="54">
         <f t="shared" si="0"/>
-        <v>30.602249999999998</v>
+        <v>30.893699999999999</v>
       </c>
       <c r="AF7" s="54">
         <f t="shared" si="0"/>
-        <v>33.474000000000004</v>
+        <v>33.7928</v>
       </c>
       <c r="AG7" s="54">
         <f t="shared" si="0"/>
-        <v>67.603200000000015</v>
+        <v>68.247040000000013</v>
       </c>
       <c r="AH7" s="54">
         <f t="shared" si="0"/>
-        <v>28.600950000000005</v>
+        <v>28.873340000000006</v>
       </c>
       <c r="AI7" s="49"/>
     </row>
@@ -3502,111 +3502,111 @@
       </c>
       <c r="H8" s="54">
         <f>H7*1.01</f>
-        <v>2251.1731935000003</v>
+        <v>2272.6129382000004</v>
       </c>
       <c r="I8" s="54">
         <f t="shared" ref="I8:AH8" si="1">I7*1.01</f>
-        <v>30.2868195</v>
+        <v>30.575265399999999</v>
       </c>
       <c r="J8" s="54">
         <f t="shared" si="1"/>
-        <v>560.30987250000021</v>
+        <v>565.64615700000013</v>
       </c>
       <c r="K8" s="54">
         <f t="shared" si="1"/>
-        <v>108.75957750000003</v>
+        <v>109.79538300000003</v>
       </c>
       <c r="L8" s="54">
         <f t="shared" si="1"/>
-        <v>49.069334999999995</v>
+        <v>49.536661999999993</v>
       </c>
       <c r="M8" s="54">
         <f t="shared" si="1"/>
-        <v>37.153556999999999</v>
+        <v>37.507400400000002</v>
       </c>
       <c r="N8" s="54">
         <f t="shared" si="1"/>
-        <v>19.407149999999998</v>
+        <v>19.59198</v>
       </c>
       <c r="O8" s="54">
         <f t="shared" si="1"/>
-        <v>54.084439499999995</v>
+        <v>54.599529400000002</v>
       </c>
       <c r="P8" s="54">
         <f t="shared" si="1"/>
-        <v>92.749209000000008</v>
+        <v>93.632534800000016</v>
       </c>
       <c r="Q8" s="54">
         <f t="shared" si="1"/>
-        <v>36.378331500000002</v>
+        <v>36.724791799999998</v>
       </c>
       <c r="R8" s="54">
         <f t="shared" si="1"/>
-        <v>43.864400999999994</v>
+        <v>44.2821572</v>
       </c>
       <c r="S8" s="54">
         <f t="shared" si="1"/>
-        <v>79.609614000000008</v>
+        <v>80.367800800000012</v>
       </c>
       <c r="T8" s="54">
         <f t="shared" si="1"/>
-        <v>72.426847499999994</v>
+        <v>73.116627000000008</v>
       </c>
       <c r="U8" s="54">
         <f t="shared" si="1"/>
-        <v>60.976629000000003</v>
+        <v>61.557358799999996</v>
       </c>
       <c r="V8" s="54">
         <f t="shared" si="1"/>
-        <v>274.10531400000002</v>
+        <v>276.71584080000002</v>
       </c>
       <c r="W8" s="54">
         <f t="shared" si="1"/>
-        <v>77.704955999999996</v>
+        <v>78.445003199999988</v>
       </c>
       <c r="X8" s="54">
         <f t="shared" si="1"/>
-        <v>93.591245999999998</v>
+        <v>94.482591200000002</v>
       </c>
       <c r="Y8" s="54">
         <f t="shared" si="1"/>
-        <v>83.819799000000003</v>
+        <v>84.61808280000001</v>
       </c>
       <c r="Z8" s="54">
         <f t="shared" si="1"/>
-        <v>61.275689999999997</v>
+        <v>61.859267999999993</v>
       </c>
       <c r="AA8" s="54">
         <f t="shared" si="1"/>
-        <v>138.18739200000005</v>
+        <v>139.50346240000005</v>
       </c>
       <c r="AB8" s="54">
         <f t="shared" si="1"/>
-        <v>15.7791795</v>
+        <v>15.929457400000002</v>
       </c>
       <c r="AC8" s="54">
         <f t="shared" si="1"/>
-        <v>65.061674999999994</v>
+        <v>65.681309999999996</v>
       </c>
       <c r="AD8" s="54">
         <f t="shared" si="1"/>
-        <v>34.688955000000007</v>
+        <v>35.019326000000014</v>
       </c>
       <c r="AE8" s="54">
         <f t="shared" si="1"/>
-        <v>30.908272499999999</v>
+        <v>31.202636999999999</v>
       </c>
       <c r="AF8" s="54">
         <f t="shared" si="1"/>
-        <v>33.808740000000007</v>
+        <v>34.130727999999998</v>
       </c>
       <c r="AG8" s="54">
         <f t="shared" si="1"/>
-        <v>68.279232000000022</v>
+        <v>68.929510400000012</v>
       </c>
       <c r="AH8" s="54">
         <f t="shared" si="1"/>
-        <v>28.886959500000003</v>
+        <v>29.162073400000008</v>
       </c>
     </row>
     <row r="9" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.3">
@@ -3618,111 +3618,111 @@
       </c>
       <c r="H9" s="54">
         <f>H8*1.05</f>
-        <v>2363.7318531750002</v>
+        <v>2386.2435851100004</v>
       </c>
       <c r="I9" s="54">
         <f t="shared" ref="I9:AH9" si="2">I8*1.05</f>
-        <v>31.801160475</v>
+        <v>32.104028669999998</v>
       </c>
       <c r="J9" s="54">
         <f t="shared" si="2"/>
-        <v>588.3253661250003</v>
+        <v>593.92846485000018</v>
       </c>
       <c r="K9" s="54">
         <f t="shared" si="2"/>
-        <v>114.19755637500005</v>
+        <v>115.28515215000003</v>
       </c>
       <c r="L9" s="54">
         <f t="shared" si="2"/>
-        <v>51.522801749999999</v>
+        <v>52.013495099999993</v>
       </c>
       <c r="M9" s="54">
         <f t="shared" si="2"/>
-        <v>39.011234850000001</v>
+        <v>39.38277042</v>
       </c>
       <c r="N9" s="54">
         <f t="shared" si="2"/>
-        <v>20.3775075</v>
+        <v>20.571579</v>
       </c>
       <c r="O9" s="54">
         <f t="shared" si="2"/>
-        <v>56.788661474999998</v>
+        <v>57.329505870000006</v>
       </c>
       <c r="P9" s="54">
         <f t="shared" si="2"/>
-        <v>97.386669450000014</v>
+        <v>98.314161540000015</v>
       </c>
       <c r="Q9" s="54">
         <f t="shared" si="2"/>
-        <v>38.197248075000005</v>
+        <v>38.561031389999997</v>
       </c>
       <c r="R9" s="54">
         <f t="shared" si="2"/>
-        <v>46.057621049999995</v>
+        <v>46.496265059999999</v>
       </c>
       <c r="S9" s="54">
         <f t="shared" si="2"/>
-        <v>83.590094700000009</v>
+        <v>84.386190840000012</v>
       </c>
       <c r="T9" s="54">
         <f t="shared" si="2"/>
-        <v>76.048189874999991</v>
+        <v>76.772458350000008</v>
       </c>
       <c r="U9" s="54">
         <f t="shared" si="2"/>
-        <v>64.025460450000011</v>
+        <v>64.635226739999993</v>
       </c>
       <c r="V9" s="54">
         <f t="shared" si="2"/>
-        <v>287.81057970000006</v>
+        <v>290.55163284000002</v>
       </c>
       <c r="W9" s="54">
         <f t="shared" si="2"/>
-        <v>81.590203799999998</v>
+        <v>82.367253359999992</v>
       </c>
       <c r="X9" s="54">
         <f t="shared" si="2"/>
-        <v>98.270808299999999</v>
+        <v>99.20672076000001</v>
       </c>
       <c r="Y9" s="54">
         <f t="shared" si="2"/>
-        <v>88.010788950000006</v>
+        <v>88.848986940000017</v>
       </c>
       <c r="Z9" s="54">
         <f t="shared" si="2"/>
-        <v>64.339474499999994</v>
+        <v>64.952231400000002</v>
       </c>
       <c r="AA9" s="54">
         <f t="shared" si="2"/>
-        <v>145.09676160000006</v>
+        <v>146.47863552000007</v>
       </c>
       <c r="AB9" s="54">
         <f t="shared" si="2"/>
-        <v>16.568138475000001</v>
+        <v>16.725930270000003</v>
       </c>
       <c r="AC9" s="54">
         <f t="shared" si="2"/>
-        <v>68.314758749999996</v>
+        <v>68.965375499999993</v>
       </c>
       <c r="AD9" s="54">
         <f t="shared" si="2"/>
-        <v>36.423402750000008</v>
+        <v>36.770292300000015</v>
       </c>
       <c r="AE9" s="54">
         <f t="shared" si="2"/>
-        <v>32.453686124999997</v>
+        <v>32.76276885</v>
       </c>
       <c r="AF9" s="54">
         <f t="shared" si="2"/>
-        <v>35.49917700000001</v>
+        <v>35.837264400000002</v>
       </c>
       <c r="AG9" s="54">
         <f t="shared" si="2"/>
-        <v>71.693193600000029</v>
+        <v>72.375985920000019</v>
       </c>
       <c r="AH9" s="54">
         <f t="shared" si="2"/>
-        <v>30.331307475000006</v>
+        <v>30.620177070000011</v>
       </c>
     </row>
     <row r="10" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.3">
@@ -3734,111 +3734,111 @@
       </c>
       <c r="H10" s="54">
         <f>H9*1.12</f>
-        <v>2647.3796755560006</v>
+        <v>2672.5928153232007</v>
       </c>
       <c r="I10" s="54">
         <f t="shared" ref="I10:AH10" si="3">I9*1.12</f>
-        <v>35.617299732000006</v>
+        <v>35.956512110399999</v>
       </c>
       <c r="J10" s="54">
         <f t="shared" si="3"/>
-        <v>658.92441006000035</v>
+        <v>665.19988063200026</v>
       </c>
       <c r="K10" s="54">
         <f t="shared" si="3"/>
-        <v>127.90126314000007</v>
+        <v>129.11937040800004</v>
       </c>
       <c r="L10" s="54">
         <f t="shared" si="3"/>
-        <v>57.705537960000008</v>
+        <v>58.255114511999999</v>
       </c>
       <c r="M10" s="54">
         <f t="shared" si="3"/>
-        <v>43.692583032000009</v>
+        <v>44.108702870400002</v>
       </c>
       <c r="N10" s="54">
         <f t="shared" si="3"/>
-        <v>22.822808400000003</v>
+        <v>23.040168480000002</v>
       </c>
       <c r="O10" s="54">
         <f t="shared" si="3"/>
-        <v>63.603300852000004</v>
+        <v>64.209046574400006</v>
       </c>
       <c r="P10" s="54">
         <f t="shared" si="3"/>
-        <v>109.07306978400003</v>
+        <v>110.11186092480003</v>
       </c>
       <c r="Q10" s="54">
         <f t="shared" si="3"/>
-        <v>42.780917844000008</v>
+        <v>43.1883551568</v>
       </c>
       <c r="R10" s="54">
         <f t="shared" si="3"/>
-        <v>51.584535576</v>
+        <v>52.075816867200004</v>
       </c>
       <c r="S10" s="54">
         <f t="shared" si="3"/>
-        <v>93.620906064000025</v>
+        <v>94.512533740800023</v>
       </c>
       <c r="T10" s="54">
         <f t="shared" si="3"/>
-        <v>85.173972660000004</v>
+        <v>85.985153352000012</v>
       </c>
       <c r="U10" s="54">
         <f t="shared" si="3"/>
-        <v>71.708515704000021</v>
+        <v>72.391453948800006</v>
       </c>
       <c r="V10" s="54">
         <f t="shared" si="3"/>
-        <v>322.3478492640001</v>
+        <v>325.41782878080005</v>
       </c>
       <c r="W10" s="54">
         <f t="shared" si="3"/>
-        <v>91.381028256000008</v>
+        <v>92.251323763200006</v>
       </c>
       <c r="X10" s="54">
         <f t="shared" si="3"/>
-        <v>110.06330529600001</v>
+        <v>111.11152725120002</v>
       </c>
       <c r="Y10" s="54">
         <f t="shared" si="3"/>
-        <v>98.572083624000015</v>
+        <v>99.510865372800026</v>
       </c>
       <c r="Z10" s="54">
         <f t="shared" si="3"/>
-        <v>72.060211440000003</v>
+        <v>72.746499168000014</v>
       </c>
       <c r="AA10" s="54">
         <f t="shared" si="3"/>
-        <v>162.50837299200009</v>
+        <v>164.0560717824001</v>
       </c>
       <c r="AB10" s="54">
         <f t="shared" si="3"/>
-        <v>18.556315092000002</v>
+        <v>18.733041902400004</v>
       </c>
       <c r="AC10" s="54">
         <f t="shared" si="3"/>
-        <v>76.512529799999996</v>
+        <v>77.241220560000002</v>
       </c>
       <c r="AD10" s="54">
         <f t="shared" si="3"/>
-        <v>40.794211080000011</v>
+        <v>41.182727376000024</v>
       </c>
       <c r="AE10" s="54">
         <f t="shared" si="3"/>
-        <v>36.348128459999998</v>
+        <v>36.694301112000005</v>
       </c>
       <c r="AF10" s="54">
         <f t="shared" si="3"/>
-        <v>39.759078240000015</v>
+        <v>40.137736128000007</v>
       </c>
       <c r="AG10" s="54">
         <f t="shared" si="3"/>
-        <v>80.296376832000036</v>
+        <v>81.061104230400034</v>
       </c>
       <c r="AH10" s="54">
         <f t="shared" si="3"/>
-        <v>33.971064372000008</v>
+        <v>34.294598318400013</v>
       </c>
     </row>
     <row r="11" spans="1:35" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -3850,111 +3850,111 @@
       </c>
       <c r="H11" s="54">
         <f>H7*1.35</f>
-        <v>3008.9938725000006</v>
+        <v>3037.6509570000007</v>
       </c>
       <c r="I11" s="54">
         <f t="shared" ref="I11:AH11" si="4">I7*1.35</f>
-        <v>40.4823825</v>
+        <v>40.867929000000004</v>
       </c>
       <c r="J11" s="54">
         <f t="shared" si="4"/>
-        <v>748.92903750000039</v>
+        <v>756.06169500000021</v>
       </c>
       <c r="K11" s="54">
         <f t="shared" si="4"/>
-        <v>145.37171250000006</v>
+        <v>146.75620500000005</v>
       </c>
       <c r="L11" s="54">
         <f t="shared" si="4"/>
-        <v>65.587724999999992</v>
+        <v>66.212369999999993</v>
       </c>
       <c r="M11" s="54">
         <f t="shared" si="4"/>
-        <v>49.660695000000004</v>
+        <v>50.133654000000007</v>
       </c>
       <c r="N11" s="54">
         <f t="shared" si="4"/>
-        <v>25.940249999999995</v>
+        <v>26.1873</v>
       </c>
       <c r="O11" s="54">
         <f t="shared" si="4"/>
-        <v>72.291082500000002</v>
+        <v>72.979568999999998</v>
       </c>
       <c r="P11" s="54">
         <f t="shared" si="4"/>
-        <v>123.971715</v>
+        <v>125.15239800000002</v>
       </c>
       <c r="Q11" s="54">
         <f t="shared" si="4"/>
-        <v>48.624502499999998</v>
+        <v>49.087592999999998</v>
       </c>
       <c r="R11" s="54">
         <f t="shared" si="4"/>
-        <v>58.630634999999998</v>
+        <v>59.189022000000001</v>
       </c>
       <c r="S11" s="54">
         <f t="shared" si="4"/>
-        <v>106.40889000000003</v>
+        <v>107.42230800000003</v>
       </c>
       <c r="T11" s="54">
         <f t="shared" si="4"/>
-        <v>96.808162500000009</v>
+        <v>97.730145000000007</v>
       </c>
       <c r="U11" s="54">
         <f t="shared" si="4"/>
-        <v>81.503415000000004</v>
+        <v>82.279638000000006</v>
       </c>
       <c r="V11" s="54">
         <f t="shared" si="4"/>
-        <v>366.37839000000008</v>
+        <v>369.86770800000005</v>
       </c>
       <c r="W11" s="54">
         <f t="shared" si="4"/>
-        <v>103.86306</v>
+        <v>104.852232</v>
       </c>
       <c r="X11" s="54">
         <f t="shared" si="4"/>
-        <v>125.09721</v>
+        <v>126.28861200000001</v>
       </c>
       <c r="Y11" s="54">
         <f t="shared" si="4"/>
-        <v>112.03636500000002</v>
+        <v>113.10337800000002</v>
       </c>
       <c r="Z11" s="54">
         <f t="shared" si="4"/>
-        <v>81.903149999999997</v>
+        <v>82.683179999999993</v>
       </c>
       <c r="AA11" s="54">
         <f t="shared" si="4"/>
-        <v>184.70592000000008</v>
+        <v>186.46502400000006</v>
       </c>
       <c r="AB11" s="54">
         <f t="shared" si="4"/>
-        <v>21.090982499999999</v>
+        <v>21.291849000000003</v>
       </c>
       <c r="AC11" s="54">
         <f t="shared" si="4"/>
-        <v>86.963624999999993</v>
+        <v>87.791849999999997</v>
       </c>
       <c r="AD11" s="54">
         <f t="shared" si="4"/>
-        <v>46.366425000000014</v>
+        <v>46.808010000000017</v>
       </c>
       <c r="AE11" s="54">
         <f t="shared" si="4"/>
-        <v>41.3130375</v>
+        <v>41.706495000000004</v>
       </c>
       <c r="AF11" s="54">
         <f t="shared" si="4"/>
-        <v>45.189900000000009</v>
+        <v>45.620280000000001</v>
       </c>
       <c r="AG11" s="54">
         <f t="shared" si="4"/>
-        <v>91.264320000000026</v>
+        <v>92.133504000000016</v>
       </c>
       <c r="AH11" s="54">
         <f t="shared" si="4"/>
-        <v>38.611282500000009</v>
+        <v>38.979009000000012</v>
       </c>
       <c r="AI11" s="49"/>
     </row>

</xml_diff>